<commit_message>
Bat para instalar fórmula de escrever por extenso
</commit_message>
<xml_diff>
--- a/Controle Domestica.xlsx
+++ b/Controle Domestica.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
-  <workbookPr codeName="EstaPastaDeTrabalho" defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr codeName="EstaPastaDeTrabalho"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\pln_controle_domestica\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\ExcelGuru-controle-domestica\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -36,7 +36,7 @@
     <definedName name="QTD_VALETRANSPORTE">'Dados Gerais'!$B$3</definedName>
     <definedName name="VALOR_VALETRANSPORTE">'Dados Gerais'!$B$2</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="106">
   <si>
     <t>#</t>
   </si>
@@ -399,7 +399,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="5">
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="[$-416]d\-mmm;@"/>
@@ -1011,83 +1011,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1099,9 +1022,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1132,6 +1052,86 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1139,20 +1139,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="55">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFDADA"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1167,7 +1153,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1187,7 +1172,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1207,7 +1191,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1227,7 +1210,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1247,7 +1229,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1267,7 +1248,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1287,7 +1267,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="164" formatCode="[$-416]d\-mmm;@"/>
@@ -1307,7 +1286,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1326,10 +1304,23 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFDADA"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="166" formatCode="[h]:mm"/>
@@ -1398,7 +1389,6 @@
         <sz val="14"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1413,7 +1403,6 @@
         <sz val="14"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1428,7 +1417,6 @@
         <sz val="14"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1443,7 +1431,6 @@
         <sz val="14"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1577,7 +1564,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BA63870B-E726-47E2-A325-54207960A327}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BA63870B-E726-47E2-A325-54207960A327}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1586,13 +1573,13 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
             <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
-              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId3"/>
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" xmlns="" r:embed="rId3"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1636,7 +1623,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C4A448C-1BDE-4308-8D89-CF00FF4129D5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9C4A448C-1BDE-4308-8D89-CF00FF4129D5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1645,13 +1632,13 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
             <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
-              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId3"/>
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" xmlns="" r:embed="rId3"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1781,19 +1768,19 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="tbCalculoValeTransporte" displayName="tbCalculoValeTransporte" ref="B5:H36" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="tbCalculoValeTransporte" displayName="tbCalculoValeTransporte" ref="B5:H36" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <tableColumns count="7">
-    <tableColumn id="1" name="Data" dataDxfId="8"/>
-    <tableColumn id="2" name="Dia" dataDxfId="7">
+    <tableColumn id="1" name="Data" dataDxfId="6"/>
+    <tableColumn id="2" name="Dia" dataDxfId="5">
       <calculatedColumnFormula>TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"ddd")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Trabalhou em dia não útil?" dataDxfId="6"/>
-    <tableColumn id="4" name="Custo Extra?" dataDxfId="5" dataCellStyle="Moeda"/>
-    <tableColumn id="6" name="Faltou no dia?" dataDxfId="4" dataCellStyle="Moeda"/>
-    <tableColumn id="5" name="sts" dataDxfId="3">
+    <tableColumn id="3" name="Trabalhou em dia não útil?" dataDxfId="4"/>
+    <tableColumn id="4" name="Custo Extra?" dataDxfId="3" dataCellStyle="Moeda"/>
+    <tableColumn id="6" name="Faltou no dia?" dataDxfId="2" dataCellStyle="Moeda"/>
+    <tableColumn id="5" name="sts" dataDxfId="1">
       <calculatedColumnFormula>IF(tbCalculoValeTransporte[[#This Row],[Data]]&lt;&gt;"",IF(AND(tbCalculoValeTransporte[[#This Row],[Trabalhou em dia não útil?]]="Sim",tbCalculoValeTransporte[[#This Row],[Faltou no dia?]]="Sim"),-1,IF(VLOOKUP(tbCalculoValeTransporte[[#This Row],[Dia]],tbJornada[[Abreviatura]:[É dia util?]],2,FALSE)="Sim",IF(ISERROR(VLOOKUP(TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"dd-mmm"),tbFeriados[Dia / Mês],1,FALSE)),IF(NOT(tbCalculoValeTransporte[[#This Row],[Faltou no dia?]]="Sim"),1,0),0),IF(tbCalculoValeTransporte[[#This Row],[Trabalhou em dia não útil?]]="Sim",1,0))),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="PRINT" dataDxfId="2">
+    <tableColumn id="7" name="PRINT" dataDxfId="0">
       <calculatedColumnFormula>IF(tbCalculoValeTransporte[[#This Row],[sts]]=1,TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"dd-mmm")&amp;"-"&amp;$D$3,"")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2826,8 +2813,8 @@
   <dimension ref="B1:K36"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D34" sqref="D34"/>
+      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2845,18 +2832,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="F1" s="50" t="s">
+      <c r="F1" s="76" t="s">
         <v>82</v>
       </c>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
     </row>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="72" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="47"/>
+      <c r="C2" s="73"/>
       <c r="D2" s="17" t="s">
         <v>41</v>
       </c>
@@ -2866,17 +2853,13 @@
       <c r="F2" s="32"/>
     </row>
     <row r="3" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="48" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="49"/>
-      <c r="D3" s="19">
-        <v>2017</v>
-      </c>
+      <c r="B3" s="74"/>
+      <c r="C3" s="75"/>
+      <c r="D3" s="19"/>
       <c r="E3" s="20"/>
-      <c r="F3" s="27">
+      <c r="F3" s="27" t="str">
         <f>IF(ISERROR(DATEVALUE(IF(E3&lt;&gt;"",E3,1)&amp;"-"&amp;B3&amp;"-"&amp;D3)),"",DATEVALUE(IF(E3&lt;&gt;"",E3,1)&amp;"-"&amp;B3&amp;"-"&amp;D3))</f>
-        <v>42736</v>
+        <v/>
       </c>
       <c r="J3" s="31"/>
       <c r="K3" s="28" t="s">
@@ -2913,20 +2896,20 @@
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="21">
+      <c r="B6" s="21" t="str">
         <f>IF(ISERROR($F$3),"",$F$3)</f>
-        <v>42736</v>
+        <v/>
       </c>
       <c r="C6" s="5" t="str">
         <f>TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"ddd")</f>
-        <v>dom</v>
+        <v/>
       </c>
       <c r="D6" s="35"/>
       <c r="E6" s="36"/>
       <c r="F6" s="36"/>
-      <c r="G6" s="33">
+      <c r="G6" s="33" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[Data]]&lt;&gt;"",IF(AND(tbCalculoValeTransporte[[#This Row],[Trabalhou em dia não útil?]]="Sim",tbCalculoValeTransporte[[#This Row],[Faltou no dia?]]="Sim"),-1,IF(VLOOKUP(tbCalculoValeTransporte[[#This Row],[Dia]],tbJornada[[Abreviatura]:[É dia util?]],2,FALSE)="Sim",IF(ISERROR(VLOOKUP(TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"dd-mmm"),tbFeriados[Dia / Mês],1,FALSE)),IF(NOT(tbCalculoValeTransporte[[#This Row],[Faltou no dia?]]="Sim"),1,0),0),IF(tbCalculoValeTransporte[[#This Row],[Trabalhou em dia não útil?]]="Sim",1,0))),"")</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="H6" s="5" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[sts]]=1,TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"dd-mmm")&amp;"-"&amp;$D$3,"")</f>
@@ -2938,24 +2921,24 @@
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="21">
+      <c r="B7" s="21" t="str">
         <f>IF(B6&lt;&gt;"",IF(DAY(B6+1)=IF($E$3&lt;&gt;"",$E$3,1),"",B6+1),"")</f>
-        <v>42737</v>
+        <v/>
       </c>
       <c r="C7" s="5" t="str">
         <f>TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"ddd")</f>
-        <v>seg</v>
+        <v/>
       </c>
       <c r="D7" s="35"/>
       <c r="E7" s="36"/>
       <c r="F7" s="36"/>
-      <c r="G7" s="33">
+      <c r="G7" s="33" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[Data]]&lt;&gt;"",IF(AND(tbCalculoValeTransporte[[#This Row],[Trabalhou em dia não útil?]]="Sim",tbCalculoValeTransporte[[#This Row],[Faltou no dia?]]="Sim"),-1,IF(VLOOKUP(tbCalculoValeTransporte[[#This Row],[Dia]],tbJornada[[Abreviatura]:[É dia util?]],2,FALSE)="Sim",IF(ISERROR(VLOOKUP(TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"dd-mmm"),tbFeriados[Dia / Mês],1,FALSE)),IF(NOT(tbCalculoValeTransporte[[#This Row],[Faltou no dia?]]="Sim"),1,0),0),IF(tbCalculoValeTransporte[[#This Row],[Trabalhou em dia não útil?]]="Sim",1,0))),"")</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="H7" s="5" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[sts]]=1,TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"dd-mmm")&amp;"-"&amp;$D$3,"")</f>
-        <v>02-jan-2017</v>
+        <v/>
       </c>
       <c r="I7" s="34" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[sts]]&lt;0,"Não pode marcar como trabalhado no dia útil e faltado ao mesmo tempo","")</f>
@@ -2963,24 +2946,24 @@
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="21">
+      <c r="B8" s="21" t="str">
         <f t="shared" ref="B8:B36" si="0">IF(B7&lt;&gt;"",IF(DAY(B7+1)=IF($E$3&lt;&gt;"",$E$3,1),"",B7+1),"")</f>
-        <v>42738</v>
+        <v/>
       </c>
       <c r="C8" s="5" t="str">
         <f>TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"ddd")</f>
-        <v>ter</v>
+        <v/>
       </c>
       <c r="D8" s="35"/>
       <c r="E8" s="36"/>
       <c r="F8" s="36"/>
-      <c r="G8" s="33">
+      <c r="G8" s="33" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[Data]]&lt;&gt;"",IF(AND(tbCalculoValeTransporte[[#This Row],[Trabalhou em dia não útil?]]="Sim",tbCalculoValeTransporte[[#This Row],[Faltou no dia?]]="Sim"),-1,IF(VLOOKUP(tbCalculoValeTransporte[[#This Row],[Dia]],tbJornada[[Abreviatura]:[É dia util?]],2,FALSE)="Sim",IF(ISERROR(VLOOKUP(TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"dd-mmm"),tbFeriados[Dia / Mês],1,FALSE)),IF(NOT(tbCalculoValeTransporte[[#This Row],[Faltou no dia?]]="Sim"),1,0),0),IF(tbCalculoValeTransporte[[#This Row],[Trabalhou em dia não útil?]]="Sim",1,0))),"")</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="H8" s="5" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[sts]]=1,TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"dd-mmm")&amp;"-"&amp;$D$3,"")</f>
-        <v>03-jan-2017</v>
+        <v/>
       </c>
       <c r="I8" s="34" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[sts]]&lt;0,"Não pode marcar como trabalhado no dia útil e faltado ao mesmo tempo","")</f>
@@ -2988,24 +2971,24 @@
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="21">
+      <c r="B9" s="21" t="str">
         <f t="shared" si="0"/>
-        <v>42739</v>
+        <v/>
       </c>
       <c r="C9" s="5" t="str">
         <f>TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"ddd")</f>
-        <v>qua</v>
+        <v/>
       </c>
       <c r="D9" s="35"/>
       <c r="E9" s="36"/>
       <c r="F9" s="36"/>
-      <c r="G9" s="33">
+      <c r="G9" s="33" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[Data]]&lt;&gt;"",IF(AND(tbCalculoValeTransporte[[#This Row],[Trabalhou em dia não útil?]]="Sim",tbCalculoValeTransporte[[#This Row],[Faltou no dia?]]="Sim"),-1,IF(VLOOKUP(tbCalculoValeTransporte[[#This Row],[Dia]],tbJornada[[Abreviatura]:[É dia util?]],2,FALSE)="Sim",IF(ISERROR(VLOOKUP(TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"dd-mmm"),tbFeriados[Dia / Mês],1,FALSE)),IF(NOT(tbCalculoValeTransporte[[#This Row],[Faltou no dia?]]="Sim"),1,0),0),IF(tbCalculoValeTransporte[[#This Row],[Trabalhou em dia não útil?]]="Sim",1,0))),"")</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="H9" s="5" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[sts]]=1,TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"dd-mmm")&amp;"-"&amp;$D$3,"")</f>
-        <v>04-jan-2017</v>
+        <v/>
       </c>
       <c r="I9" s="34" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[sts]]&lt;0,"Não pode marcar como trabalhado no dia útil e faltado ao mesmo tempo","")</f>
@@ -3013,24 +2996,24 @@
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="21">
+      <c r="B10" s="21" t="str">
         <f t="shared" si="0"/>
-        <v>42740</v>
+        <v/>
       </c>
       <c r="C10" s="5" t="str">
         <f>TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"ddd")</f>
-        <v>qui</v>
+        <v/>
       </c>
       <c r="D10" s="35"/>
       <c r="E10" s="36"/>
       <c r="F10" s="36"/>
-      <c r="G10" s="33">
+      <c r="G10" s="33" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[Data]]&lt;&gt;"",IF(AND(tbCalculoValeTransporte[[#This Row],[Trabalhou em dia não útil?]]="Sim",tbCalculoValeTransporte[[#This Row],[Faltou no dia?]]="Sim"),-1,IF(VLOOKUP(tbCalculoValeTransporte[[#This Row],[Dia]],tbJornada[[Abreviatura]:[É dia util?]],2,FALSE)="Sim",IF(ISERROR(VLOOKUP(TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"dd-mmm"),tbFeriados[Dia / Mês],1,FALSE)),IF(NOT(tbCalculoValeTransporte[[#This Row],[Faltou no dia?]]="Sim"),1,0),0),IF(tbCalculoValeTransporte[[#This Row],[Trabalhou em dia não útil?]]="Sim",1,0))),"")</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="H10" s="5" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[sts]]=1,TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"dd-mmm")&amp;"-"&amp;$D$3,"")</f>
-        <v>05-jan-2017</v>
+        <v/>
       </c>
       <c r="I10" s="34" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[sts]]&lt;0,"Não pode marcar como trabalhado no dia útil e faltado ao mesmo tempo","")</f>
@@ -3038,24 +3021,24 @@
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="21">
+      <c r="B11" s="21" t="str">
         <f t="shared" si="0"/>
-        <v>42741</v>
+        <v/>
       </c>
       <c r="C11" s="5" t="str">
         <f>TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"ddd")</f>
-        <v>sex</v>
+        <v/>
       </c>
       <c r="D11" s="35"/>
       <c r="E11" s="36"/>
       <c r="F11" s="36"/>
-      <c r="G11" s="33">
+      <c r="G11" s="33" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[Data]]&lt;&gt;"",IF(AND(tbCalculoValeTransporte[[#This Row],[Trabalhou em dia não útil?]]="Sim",tbCalculoValeTransporte[[#This Row],[Faltou no dia?]]="Sim"),-1,IF(VLOOKUP(tbCalculoValeTransporte[[#This Row],[Dia]],tbJornada[[Abreviatura]:[É dia util?]],2,FALSE)="Sim",IF(ISERROR(VLOOKUP(TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"dd-mmm"),tbFeriados[Dia / Mês],1,FALSE)),IF(NOT(tbCalculoValeTransporte[[#This Row],[Faltou no dia?]]="Sim"),1,0),0),IF(tbCalculoValeTransporte[[#This Row],[Trabalhou em dia não útil?]]="Sim",1,0))),"")</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="H11" s="5" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[sts]]=1,TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"dd-mmm")&amp;"-"&amp;$D$3,"")</f>
-        <v>06-jan-2017</v>
+        <v/>
       </c>
       <c r="I11" s="34" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[sts]]&lt;0,"Não pode marcar como trabalhado no dia útil e faltado ao mesmo tempo","")</f>
@@ -3063,24 +3046,24 @@
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="21">
+      <c r="B12" s="21" t="str">
         <f t="shared" si="0"/>
-        <v>42742</v>
+        <v/>
       </c>
       <c r="C12" s="5" t="str">
         <f>TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"ddd")</f>
-        <v>sáb</v>
+        <v/>
       </c>
       <c r="D12" s="35"/>
       <c r="E12" s="36"/>
       <c r="F12" s="36"/>
-      <c r="G12" s="33">
+      <c r="G12" s="33" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[Data]]&lt;&gt;"",IF(AND(tbCalculoValeTransporte[[#This Row],[Trabalhou em dia não útil?]]="Sim",tbCalculoValeTransporte[[#This Row],[Faltou no dia?]]="Sim"),-1,IF(VLOOKUP(tbCalculoValeTransporte[[#This Row],[Dia]],tbJornada[[Abreviatura]:[É dia util?]],2,FALSE)="Sim",IF(ISERROR(VLOOKUP(TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"dd-mmm"),tbFeriados[Dia / Mês],1,FALSE)),IF(NOT(tbCalculoValeTransporte[[#This Row],[Faltou no dia?]]="Sim"),1,0),0),IF(tbCalculoValeTransporte[[#This Row],[Trabalhou em dia não útil?]]="Sim",1,0))),"")</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="H12" s="5" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[sts]]=1,TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"dd-mmm")&amp;"-"&amp;$D$3,"")</f>
-        <v>07-jan-2017</v>
+        <v/>
       </c>
       <c r="I12" s="34" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[sts]]&lt;0,"Não pode marcar como trabalhado no dia útil e faltado ao mesmo tempo","")</f>
@@ -3088,20 +3071,20 @@
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="21">
+      <c r="B13" s="21" t="str">
         <f t="shared" si="0"/>
-        <v>42743</v>
+        <v/>
       </c>
       <c r="C13" s="5" t="str">
         <f>TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"ddd")</f>
-        <v>dom</v>
+        <v/>
       </c>
       <c r="D13" s="35"/>
       <c r="E13" s="36"/>
       <c r="F13" s="36"/>
-      <c r="G13" s="33">
+      <c r="G13" s="33" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[Data]]&lt;&gt;"",IF(AND(tbCalculoValeTransporte[[#This Row],[Trabalhou em dia não útil?]]="Sim",tbCalculoValeTransporte[[#This Row],[Faltou no dia?]]="Sim"),-1,IF(VLOOKUP(tbCalculoValeTransporte[[#This Row],[Dia]],tbJornada[[Abreviatura]:[É dia util?]],2,FALSE)="Sim",IF(ISERROR(VLOOKUP(TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"dd-mmm"),tbFeriados[Dia / Mês],1,FALSE)),IF(NOT(tbCalculoValeTransporte[[#This Row],[Faltou no dia?]]="Sim"),1,0),0),IF(tbCalculoValeTransporte[[#This Row],[Trabalhou em dia não útil?]]="Sim",1,0))),"")</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="H13" s="5" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[sts]]=1,TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"dd-mmm")&amp;"-"&amp;$D$3,"")</f>
@@ -3113,24 +3096,24 @@
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="21">
+      <c r="B14" s="21" t="str">
         <f t="shared" si="0"/>
-        <v>42744</v>
+        <v/>
       </c>
       <c r="C14" s="5" t="str">
         <f>TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"ddd")</f>
-        <v>seg</v>
+        <v/>
       </c>
       <c r="D14" s="35"/>
       <c r="E14" s="36"/>
       <c r="F14" s="36"/>
-      <c r="G14" s="33">
+      <c r="G14" s="33" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[Data]]&lt;&gt;"",IF(AND(tbCalculoValeTransporte[[#This Row],[Trabalhou em dia não útil?]]="Sim",tbCalculoValeTransporte[[#This Row],[Faltou no dia?]]="Sim"),-1,IF(VLOOKUP(tbCalculoValeTransporte[[#This Row],[Dia]],tbJornada[[Abreviatura]:[É dia util?]],2,FALSE)="Sim",IF(ISERROR(VLOOKUP(TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"dd-mmm"),tbFeriados[Dia / Mês],1,FALSE)),IF(NOT(tbCalculoValeTransporte[[#This Row],[Faltou no dia?]]="Sim"),1,0),0),IF(tbCalculoValeTransporte[[#This Row],[Trabalhou em dia não útil?]]="Sim",1,0))),"")</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="H14" s="5" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[sts]]=1,TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"dd-mmm")&amp;"-"&amp;$D$3,"")</f>
-        <v>09-jan-2017</v>
+        <v/>
       </c>
       <c r="I14" s="34" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[sts]]&lt;0,"Não pode marcar como trabalhado no dia útil e faltado ao mesmo tempo","")</f>
@@ -3138,24 +3121,24 @@
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="21">
+      <c r="B15" s="21" t="str">
         <f t="shared" si="0"/>
-        <v>42745</v>
+        <v/>
       </c>
       <c r="C15" s="5" t="str">
         <f>TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"ddd")</f>
-        <v>ter</v>
+        <v/>
       </c>
       <c r="D15" s="35"/>
       <c r="E15" s="36"/>
       <c r="F15" s="36"/>
-      <c r="G15" s="33">
+      <c r="G15" s="33" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[Data]]&lt;&gt;"",IF(AND(tbCalculoValeTransporte[[#This Row],[Trabalhou em dia não útil?]]="Sim",tbCalculoValeTransporte[[#This Row],[Faltou no dia?]]="Sim"),-1,IF(VLOOKUP(tbCalculoValeTransporte[[#This Row],[Dia]],tbJornada[[Abreviatura]:[É dia util?]],2,FALSE)="Sim",IF(ISERROR(VLOOKUP(TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"dd-mmm"),tbFeriados[Dia / Mês],1,FALSE)),IF(NOT(tbCalculoValeTransporte[[#This Row],[Faltou no dia?]]="Sim"),1,0),0),IF(tbCalculoValeTransporte[[#This Row],[Trabalhou em dia não útil?]]="Sim",1,0))),"")</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="H15" s="5" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[sts]]=1,TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"dd-mmm")&amp;"-"&amp;$D$3,"")</f>
-        <v>10-jan-2017</v>
+        <v/>
       </c>
       <c r="I15" s="34" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[sts]]&lt;0,"Não pode marcar como trabalhado no dia útil e faltado ao mesmo tempo","")</f>
@@ -3163,24 +3146,24 @@
       </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="21">
+      <c r="B16" s="21" t="str">
         <f t="shared" si="0"/>
-        <v>42746</v>
+        <v/>
       </c>
       <c r="C16" s="5" t="str">
         <f>TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"ddd")</f>
-        <v>qua</v>
+        <v/>
       </c>
       <c r="D16" s="35"/>
       <c r="E16" s="36"/>
       <c r="F16" s="36"/>
-      <c r="G16" s="33">
+      <c r="G16" s="33" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[Data]]&lt;&gt;"",IF(AND(tbCalculoValeTransporte[[#This Row],[Trabalhou em dia não útil?]]="Sim",tbCalculoValeTransporte[[#This Row],[Faltou no dia?]]="Sim"),-1,IF(VLOOKUP(tbCalculoValeTransporte[[#This Row],[Dia]],tbJornada[[Abreviatura]:[É dia util?]],2,FALSE)="Sim",IF(ISERROR(VLOOKUP(TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"dd-mmm"),tbFeriados[Dia / Mês],1,FALSE)),IF(NOT(tbCalculoValeTransporte[[#This Row],[Faltou no dia?]]="Sim"),1,0),0),IF(tbCalculoValeTransporte[[#This Row],[Trabalhou em dia não útil?]]="Sim",1,0))),"")</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="H16" s="5" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[sts]]=1,TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"dd-mmm")&amp;"-"&amp;$D$3,"")</f>
-        <v>11-jan-2017</v>
+        <v/>
       </c>
       <c r="I16" s="34" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[sts]]&lt;0,"Não pode marcar como trabalhado no dia útil e faltado ao mesmo tempo","")</f>
@@ -3188,24 +3171,24 @@
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="21">
+      <c r="B17" s="21" t="str">
         <f t="shared" si="0"/>
-        <v>42747</v>
+        <v/>
       </c>
       <c r="C17" s="5" t="str">
         <f>TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"ddd")</f>
-        <v>qui</v>
+        <v/>
       </c>
       <c r="D17" s="35"/>
       <c r="E17" s="36"/>
       <c r="F17" s="36"/>
-      <c r="G17" s="33">
+      <c r="G17" s="33" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[Data]]&lt;&gt;"",IF(AND(tbCalculoValeTransporte[[#This Row],[Trabalhou em dia não útil?]]="Sim",tbCalculoValeTransporte[[#This Row],[Faltou no dia?]]="Sim"),-1,IF(VLOOKUP(tbCalculoValeTransporte[[#This Row],[Dia]],tbJornada[[Abreviatura]:[É dia util?]],2,FALSE)="Sim",IF(ISERROR(VLOOKUP(TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"dd-mmm"),tbFeriados[Dia / Mês],1,FALSE)),IF(NOT(tbCalculoValeTransporte[[#This Row],[Faltou no dia?]]="Sim"),1,0),0),IF(tbCalculoValeTransporte[[#This Row],[Trabalhou em dia não útil?]]="Sim",1,0))),"")</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="H17" s="5" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[sts]]=1,TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"dd-mmm")&amp;"-"&amp;$D$3,"")</f>
-        <v>12-jan-2017</v>
+        <v/>
       </c>
       <c r="I17" s="34" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[sts]]&lt;0,"Não pode marcar como trabalhado no dia útil e faltado ao mesmo tempo","")</f>
@@ -3213,24 +3196,24 @@
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B18" s="21">
+      <c r="B18" s="21" t="str">
         <f t="shared" si="0"/>
-        <v>42748</v>
+        <v/>
       </c>
       <c r="C18" s="5" t="str">
         <f>TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"ddd")</f>
-        <v>sex</v>
+        <v/>
       </c>
       <c r="D18" s="35"/>
       <c r="E18" s="36"/>
       <c r="F18" s="36"/>
-      <c r="G18" s="33">
+      <c r="G18" s="33" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[Data]]&lt;&gt;"",IF(AND(tbCalculoValeTransporte[[#This Row],[Trabalhou em dia não útil?]]="Sim",tbCalculoValeTransporte[[#This Row],[Faltou no dia?]]="Sim"),-1,IF(VLOOKUP(tbCalculoValeTransporte[[#This Row],[Dia]],tbJornada[[Abreviatura]:[É dia util?]],2,FALSE)="Sim",IF(ISERROR(VLOOKUP(TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"dd-mmm"),tbFeriados[Dia / Mês],1,FALSE)),IF(NOT(tbCalculoValeTransporte[[#This Row],[Faltou no dia?]]="Sim"),1,0),0),IF(tbCalculoValeTransporte[[#This Row],[Trabalhou em dia não útil?]]="Sim",1,0))),"")</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="H18" s="5" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[sts]]=1,TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"dd-mmm")&amp;"-"&amp;$D$3,"")</f>
-        <v>13-jan-2017</v>
+        <v/>
       </c>
       <c r="I18" s="34" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[sts]]&lt;0,"Não pode marcar como trabalhado no dia útil e faltado ao mesmo tempo","")</f>
@@ -3238,24 +3221,24 @@
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="21">
+      <c r="B19" s="21" t="str">
         <f t="shared" si="0"/>
-        <v>42749</v>
+        <v/>
       </c>
       <c r="C19" s="5" t="str">
         <f>TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"ddd")</f>
-        <v>sáb</v>
+        <v/>
       </c>
       <c r="D19" s="35"/>
       <c r="E19" s="36"/>
       <c r="F19" s="36"/>
-      <c r="G19" s="33">
+      <c r="G19" s="33" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[Data]]&lt;&gt;"",IF(AND(tbCalculoValeTransporte[[#This Row],[Trabalhou em dia não útil?]]="Sim",tbCalculoValeTransporte[[#This Row],[Faltou no dia?]]="Sim"),-1,IF(VLOOKUP(tbCalculoValeTransporte[[#This Row],[Dia]],tbJornada[[Abreviatura]:[É dia util?]],2,FALSE)="Sim",IF(ISERROR(VLOOKUP(TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"dd-mmm"),tbFeriados[Dia / Mês],1,FALSE)),IF(NOT(tbCalculoValeTransporte[[#This Row],[Faltou no dia?]]="Sim"),1,0),0),IF(tbCalculoValeTransporte[[#This Row],[Trabalhou em dia não útil?]]="Sim",1,0))),"")</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="H19" s="5" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[sts]]=1,TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"dd-mmm")&amp;"-"&amp;$D$3,"")</f>
-        <v>14-jan-2017</v>
+        <v/>
       </c>
       <c r="I19" s="34" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[sts]]&lt;0,"Não pode marcar como trabalhado no dia útil e faltado ao mesmo tempo","")</f>
@@ -3263,20 +3246,20 @@
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B20" s="21">
+      <c r="B20" s="21" t="str">
         <f t="shared" si="0"/>
-        <v>42750</v>
+        <v/>
       </c>
       <c r="C20" s="5" t="str">
         <f>TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"ddd")</f>
-        <v>dom</v>
+        <v/>
       </c>
       <c r="D20" s="35"/>
       <c r="E20" s="36"/>
       <c r="F20" s="36"/>
-      <c r="G20" s="33">
+      <c r="G20" s="33" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[Data]]&lt;&gt;"",IF(AND(tbCalculoValeTransporte[[#This Row],[Trabalhou em dia não útil?]]="Sim",tbCalculoValeTransporte[[#This Row],[Faltou no dia?]]="Sim"),-1,IF(VLOOKUP(tbCalculoValeTransporte[[#This Row],[Dia]],tbJornada[[Abreviatura]:[É dia util?]],2,FALSE)="Sim",IF(ISERROR(VLOOKUP(TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"dd-mmm"),tbFeriados[Dia / Mês],1,FALSE)),IF(NOT(tbCalculoValeTransporte[[#This Row],[Faltou no dia?]]="Sim"),1,0),0),IF(tbCalculoValeTransporte[[#This Row],[Trabalhou em dia não útil?]]="Sim",1,0))),"")</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="H20" s="5" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[sts]]=1,TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"dd-mmm")&amp;"-"&amp;$D$3,"")</f>
@@ -3288,24 +3271,24 @@
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B21" s="21">
+      <c r="B21" s="21" t="str">
         <f t="shared" si="0"/>
-        <v>42751</v>
+        <v/>
       </c>
       <c r="C21" s="5" t="str">
         <f>TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"ddd")</f>
-        <v>seg</v>
+        <v/>
       </c>
       <c r="D21" s="35"/>
       <c r="E21" s="36"/>
       <c r="F21" s="36"/>
-      <c r="G21" s="33">
+      <c r="G21" s="33" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[Data]]&lt;&gt;"",IF(AND(tbCalculoValeTransporte[[#This Row],[Trabalhou em dia não útil?]]="Sim",tbCalculoValeTransporte[[#This Row],[Faltou no dia?]]="Sim"),-1,IF(VLOOKUP(tbCalculoValeTransporte[[#This Row],[Dia]],tbJornada[[Abreviatura]:[É dia util?]],2,FALSE)="Sim",IF(ISERROR(VLOOKUP(TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"dd-mmm"),tbFeriados[Dia / Mês],1,FALSE)),IF(NOT(tbCalculoValeTransporte[[#This Row],[Faltou no dia?]]="Sim"),1,0),0),IF(tbCalculoValeTransporte[[#This Row],[Trabalhou em dia não útil?]]="Sim",1,0))),"")</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="H21" s="5" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[sts]]=1,TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"dd-mmm")&amp;"-"&amp;$D$3,"")</f>
-        <v>16-jan-2017</v>
+        <v/>
       </c>
       <c r="I21" s="34" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[sts]]&lt;0,"Não pode marcar como trabalhado no dia útil e faltado ao mesmo tempo","")</f>
@@ -3313,24 +3296,24 @@
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B22" s="21">
+      <c r="B22" s="21" t="str">
         <f t="shared" si="0"/>
-        <v>42752</v>
+        <v/>
       </c>
       <c r="C22" s="5" t="str">
         <f>TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"ddd")</f>
-        <v>ter</v>
+        <v/>
       </c>
       <c r="D22" s="35"/>
       <c r="E22" s="36"/>
       <c r="F22" s="36"/>
-      <c r="G22" s="33">
+      <c r="G22" s="33" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[Data]]&lt;&gt;"",IF(AND(tbCalculoValeTransporte[[#This Row],[Trabalhou em dia não útil?]]="Sim",tbCalculoValeTransporte[[#This Row],[Faltou no dia?]]="Sim"),-1,IF(VLOOKUP(tbCalculoValeTransporte[[#This Row],[Dia]],tbJornada[[Abreviatura]:[É dia util?]],2,FALSE)="Sim",IF(ISERROR(VLOOKUP(TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"dd-mmm"),tbFeriados[Dia / Mês],1,FALSE)),IF(NOT(tbCalculoValeTransporte[[#This Row],[Faltou no dia?]]="Sim"),1,0),0),IF(tbCalculoValeTransporte[[#This Row],[Trabalhou em dia não útil?]]="Sim",1,0))),"")</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="H22" s="5" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[sts]]=1,TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"dd-mmm")&amp;"-"&amp;$D$3,"")</f>
-        <v>17-jan-2017</v>
+        <v/>
       </c>
       <c r="I22" s="34" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[sts]]&lt;0,"Não pode marcar como trabalhado no dia útil e faltado ao mesmo tempo","")</f>
@@ -3338,24 +3321,24 @@
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="21">
+      <c r="B23" s="21" t="str">
         <f t="shared" si="0"/>
-        <v>42753</v>
+        <v/>
       </c>
       <c r="C23" s="5" t="str">
         <f>TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"ddd")</f>
-        <v>qua</v>
+        <v/>
       </c>
       <c r="D23" s="35"/>
       <c r="E23" s="36"/>
       <c r="F23" s="36"/>
-      <c r="G23" s="33">
+      <c r="G23" s="33" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[Data]]&lt;&gt;"",IF(AND(tbCalculoValeTransporte[[#This Row],[Trabalhou em dia não útil?]]="Sim",tbCalculoValeTransporte[[#This Row],[Faltou no dia?]]="Sim"),-1,IF(VLOOKUP(tbCalculoValeTransporte[[#This Row],[Dia]],tbJornada[[Abreviatura]:[É dia util?]],2,FALSE)="Sim",IF(ISERROR(VLOOKUP(TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"dd-mmm"),tbFeriados[Dia / Mês],1,FALSE)),IF(NOT(tbCalculoValeTransporte[[#This Row],[Faltou no dia?]]="Sim"),1,0),0),IF(tbCalculoValeTransporte[[#This Row],[Trabalhou em dia não útil?]]="Sim",1,0))),"")</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="H23" s="5" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[sts]]=1,TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"dd-mmm")&amp;"-"&amp;$D$3,"")</f>
-        <v>18-jan-2017</v>
+        <v/>
       </c>
       <c r="I23" s="34" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[sts]]&lt;0,"Não pode marcar como trabalhado no dia útil e faltado ao mesmo tempo","")</f>
@@ -3363,24 +3346,24 @@
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B24" s="21">
+      <c r="B24" s="21" t="str">
         <f t="shared" si="0"/>
-        <v>42754</v>
+        <v/>
       </c>
       <c r="C24" s="5" t="str">
         <f>TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"ddd")</f>
-        <v>qui</v>
+        <v/>
       </c>
       <c r="D24" s="35"/>
       <c r="E24" s="36"/>
       <c r="F24" s="36"/>
-      <c r="G24" s="33">
+      <c r="G24" s="33" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[Data]]&lt;&gt;"",IF(AND(tbCalculoValeTransporte[[#This Row],[Trabalhou em dia não útil?]]="Sim",tbCalculoValeTransporte[[#This Row],[Faltou no dia?]]="Sim"),-1,IF(VLOOKUP(tbCalculoValeTransporte[[#This Row],[Dia]],tbJornada[[Abreviatura]:[É dia util?]],2,FALSE)="Sim",IF(ISERROR(VLOOKUP(TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"dd-mmm"),tbFeriados[Dia / Mês],1,FALSE)),IF(NOT(tbCalculoValeTransporte[[#This Row],[Faltou no dia?]]="Sim"),1,0),0),IF(tbCalculoValeTransporte[[#This Row],[Trabalhou em dia não útil?]]="Sim",1,0))),"")</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="H24" s="5" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[sts]]=1,TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"dd-mmm")&amp;"-"&amp;$D$3,"")</f>
-        <v>19-jan-2017</v>
+        <v/>
       </c>
       <c r="I24" s="34" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[sts]]&lt;0,"Não pode marcar como trabalhado no dia útil e faltado ao mesmo tempo","")</f>
@@ -3388,24 +3371,24 @@
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B25" s="21">
+      <c r="B25" s="21" t="str">
         <f t="shared" si="0"/>
-        <v>42755</v>
+        <v/>
       </c>
       <c r="C25" s="5" t="str">
         <f>TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"ddd")</f>
-        <v>sex</v>
+        <v/>
       </c>
       <c r="D25" s="35"/>
       <c r="E25" s="36"/>
       <c r="F25" s="36"/>
-      <c r="G25" s="33">
+      <c r="G25" s="33" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[Data]]&lt;&gt;"",IF(AND(tbCalculoValeTransporte[[#This Row],[Trabalhou em dia não útil?]]="Sim",tbCalculoValeTransporte[[#This Row],[Faltou no dia?]]="Sim"),-1,IF(VLOOKUP(tbCalculoValeTransporte[[#This Row],[Dia]],tbJornada[[Abreviatura]:[É dia util?]],2,FALSE)="Sim",IF(ISERROR(VLOOKUP(TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"dd-mmm"),tbFeriados[Dia / Mês],1,FALSE)),IF(NOT(tbCalculoValeTransporte[[#This Row],[Faltou no dia?]]="Sim"),1,0),0),IF(tbCalculoValeTransporte[[#This Row],[Trabalhou em dia não útil?]]="Sim",1,0))),"")</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="H25" s="5" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[sts]]=1,TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"dd-mmm")&amp;"-"&amp;$D$3,"")</f>
-        <v>20-jan-2017</v>
+        <v/>
       </c>
       <c r="I25" s="34" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[sts]]&lt;0,"Não pode marcar como trabalhado no dia útil e faltado ao mesmo tempo","")</f>
@@ -3413,24 +3396,24 @@
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B26" s="21">
+      <c r="B26" s="21" t="str">
         <f t="shared" si="0"/>
-        <v>42756</v>
+        <v/>
       </c>
       <c r="C26" s="5" t="str">
         <f>TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"ddd")</f>
-        <v>sáb</v>
+        <v/>
       </c>
       <c r="D26" s="35"/>
       <c r="E26" s="36"/>
       <c r="F26" s="36"/>
-      <c r="G26" s="33">
+      <c r="G26" s="33" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[Data]]&lt;&gt;"",IF(AND(tbCalculoValeTransporte[[#This Row],[Trabalhou em dia não útil?]]="Sim",tbCalculoValeTransporte[[#This Row],[Faltou no dia?]]="Sim"),-1,IF(VLOOKUP(tbCalculoValeTransporte[[#This Row],[Dia]],tbJornada[[Abreviatura]:[É dia util?]],2,FALSE)="Sim",IF(ISERROR(VLOOKUP(TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"dd-mmm"),tbFeriados[Dia / Mês],1,FALSE)),IF(NOT(tbCalculoValeTransporte[[#This Row],[Faltou no dia?]]="Sim"),1,0),0),IF(tbCalculoValeTransporte[[#This Row],[Trabalhou em dia não útil?]]="Sim",1,0))),"")</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="H26" s="5" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[sts]]=1,TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"dd-mmm")&amp;"-"&amp;$D$3,"")</f>
-        <v>21-jan-2017</v>
+        <v/>
       </c>
       <c r="I26" s="34" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[sts]]&lt;0,"Não pode marcar como trabalhado no dia útil e faltado ao mesmo tempo","")</f>
@@ -3438,20 +3421,20 @@
       </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B27" s="21">
+      <c r="B27" s="21" t="str">
         <f t="shared" si="0"/>
-        <v>42757</v>
+        <v/>
       </c>
       <c r="C27" s="5" t="str">
         <f>TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"ddd")</f>
-        <v>dom</v>
+        <v/>
       </c>
       <c r="D27" s="35"/>
       <c r="E27" s="36"/>
       <c r="F27" s="36"/>
-      <c r="G27" s="33">
+      <c r="G27" s="33" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[Data]]&lt;&gt;"",IF(AND(tbCalculoValeTransporte[[#This Row],[Trabalhou em dia não útil?]]="Sim",tbCalculoValeTransporte[[#This Row],[Faltou no dia?]]="Sim"),-1,IF(VLOOKUP(tbCalculoValeTransporte[[#This Row],[Dia]],tbJornada[[Abreviatura]:[É dia util?]],2,FALSE)="Sim",IF(ISERROR(VLOOKUP(TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"dd-mmm"),tbFeriados[Dia / Mês],1,FALSE)),IF(NOT(tbCalculoValeTransporte[[#This Row],[Faltou no dia?]]="Sim"),1,0),0),IF(tbCalculoValeTransporte[[#This Row],[Trabalhou em dia não útil?]]="Sim",1,0))),"")</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="H27" s="5" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[sts]]=1,TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"dd-mmm")&amp;"-"&amp;$D$3,"")</f>
@@ -3463,24 +3446,24 @@
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B28" s="21">
+      <c r="B28" s="21" t="str">
         <f t="shared" si="0"/>
-        <v>42758</v>
+        <v/>
       </c>
       <c r="C28" s="5" t="str">
         <f>TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"ddd")</f>
-        <v>seg</v>
+        <v/>
       </c>
       <c r="D28" s="35"/>
       <c r="E28" s="36"/>
       <c r="F28" s="36"/>
-      <c r="G28" s="33">
+      <c r="G28" s="33" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[Data]]&lt;&gt;"",IF(AND(tbCalculoValeTransporte[[#This Row],[Trabalhou em dia não útil?]]="Sim",tbCalculoValeTransporte[[#This Row],[Faltou no dia?]]="Sim"),-1,IF(VLOOKUP(tbCalculoValeTransporte[[#This Row],[Dia]],tbJornada[[Abreviatura]:[É dia util?]],2,FALSE)="Sim",IF(ISERROR(VLOOKUP(TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"dd-mmm"),tbFeriados[Dia / Mês],1,FALSE)),IF(NOT(tbCalculoValeTransporte[[#This Row],[Faltou no dia?]]="Sim"),1,0),0),IF(tbCalculoValeTransporte[[#This Row],[Trabalhou em dia não útil?]]="Sim",1,0))),"")</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="H28" s="5" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[sts]]=1,TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"dd-mmm")&amp;"-"&amp;$D$3,"")</f>
-        <v>23-jan-2017</v>
+        <v/>
       </c>
       <c r="I28" s="34" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[sts]]&lt;0,"Não pode marcar como trabalhado no dia útil e faltado ao mesmo tempo","")</f>
@@ -3488,24 +3471,24 @@
       </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B29" s="21">
+      <c r="B29" s="21" t="str">
         <f t="shared" si="0"/>
-        <v>42759</v>
+        <v/>
       </c>
       <c r="C29" s="5" t="str">
         <f>TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"ddd")</f>
-        <v>ter</v>
+        <v/>
       </c>
       <c r="D29" s="35"/>
       <c r="E29" s="36"/>
       <c r="F29" s="36"/>
-      <c r="G29" s="33">
+      <c r="G29" s="33" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[Data]]&lt;&gt;"",IF(AND(tbCalculoValeTransporte[[#This Row],[Trabalhou em dia não útil?]]="Sim",tbCalculoValeTransporte[[#This Row],[Faltou no dia?]]="Sim"),-1,IF(VLOOKUP(tbCalculoValeTransporte[[#This Row],[Dia]],tbJornada[[Abreviatura]:[É dia util?]],2,FALSE)="Sim",IF(ISERROR(VLOOKUP(TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"dd-mmm"),tbFeriados[Dia / Mês],1,FALSE)),IF(NOT(tbCalculoValeTransporte[[#This Row],[Faltou no dia?]]="Sim"),1,0),0),IF(tbCalculoValeTransporte[[#This Row],[Trabalhou em dia não útil?]]="Sim",1,0))),"")</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="H29" s="5" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[sts]]=1,TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"dd-mmm")&amp;"-"&amp;$D$3,"")</f>
-        <v>24-jan-2017</v>
+        <v/>
       </c>
       <c r="I29" s="34" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[sts]]&lt;0,"Não pode marcar como trabalhado no dia útil e faltado ao mesmo tempo","")</f>
@@ -3513,24 +3496,24 @@
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B30" s="21">
+      <c r="B30" s="21" t="str">
         <f t="shared" si="0"/>
-        <v>42760</v>
+        <v/>
       </c>
       <c r="C30" s="5" t="str">
         <f>TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"ddd")</f>
-        <v>qua</v>
+        <v/>
       </c>
       <c r="D30" s="35"/>
       <c r="E30" s="36"/>
       <c r="F30" s="36"/>
-      <c r="G30" s="33">
+      <c r="G30" s="33" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[Data]]&lt;&gt;"",IF(AND(tbCalculoValeTransporte[[#This Row],[Trabalhou em dia não útil?]]="Sim",tbCalculoValeTransporte[[#This Row],[Faltou no dia?]]="Sim"),-1,IF(VLOOKUP(tbCalculoValeTransporte[[#This Row],[Dia]],tbJornada[[Abreviatura]:[É dia util?]],2,FALSE)="Sim",IF(ISERROR(VLOOKUP(TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"dd-mmm"),tbFeriados[Dia / Mês],1,FALSE)),IF(NOT(tbCalculoValeTransporte[[#This Row],[Faltou no dia?]]="Sim"),1,0),0),IF(tbCalculoValeTransporte[[#This Row],[Trabalhou em dia não útil?]]="Sim",1,0))),"")</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="H30" s="5" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[sts]]=1,TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"dd-mmm")&amp;"-"&amp;$D$3,"")</f>
-        <v>25-jan-2017</v>
+        <v/>
       </c>
       <c r="I30" s="34" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[sts]]&lt;0,"Não pode marcar como trabalhado no dia útil e faltado ao mesmo tempo","")</f>
@@ -3538,24 +3521,24 @@
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B31" s="21">
+      <c r="B31" s="21" t="str">
         <f t="shared" si="0"/>
-        <v>42761</v>
+        <v/>
       </c>
       <c r="C31" s="5" t="str">
         <f>TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"ddd")</f>
-        <v>qui</v>
+        <v/>
       </c>
       <c r="D31" s="35"/>
       <c r="E31" s="36"/>
       <c r="F31" s="36"/>
-      <c r="G31" s="33">
+      <c r="G31" s="33" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[Data]]&lt;&gt;"",IF(AND(tbCalculoValeTransporte[[#This Row],[Trabalhou em dia não útil?]]="Sim",tbCalculoValeTransporte[[#This Row],[Faltou no dia?]]="Sim"),-1,IF(VLOOKUP(tbCalculoValeTransporte[[#This Row],[Dia]],tbJornada[[Abreviatura]:[É dia util?]],2,FALSE)="Sim",IF(ISERROR(VLOOKUP(TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"dd-mmm"),tbFeriados[Dia / Mês],1,FALSE)),IF(NOT(tbCalculoValeTransporte[[#This Row],[Faltou no dia?]]="Sim"),1,0),0),IF(tbCalculoValeTransporte[[#This Row],[Trabalhou em dia não útil?]]="Sim",1,0))),"")</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="H31" s="5" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[sts]]=1,TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"dd-mmm")&amp;"-"&amp;$D$3,"")</f>
-        <v>26-jan-2017</v>
+        <v/>
       </c>
       <c r="I31" s="34" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[sts]]&lt;0,"Não pode marcar como trabalhado no dia útil e faltado ao mesmo tempo","")</f>
@@ -3563,24 +3546,24 @@
       </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B32" s="21">
+      <c r="B32" s="21" t="str">
         <f t="shared" si="0"/>
-        <v>42762</v>
+        <v/>
       </c>
       <c r="C32" s="5" t="str">
         <f>TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"ddd")</f>
-        <v>sex</v>
+        <v/>
       </c>
       <c r="D32" s="35"/>
       <c r="E32" s="36"/>
       <c r="F32" s="36"/>
-      <c r="G32" s="33">
+      <c r="G32" s="33" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[Data]]&lt;&gt;"",IF(AND(tbCalculoValeTransporte[[#This Row],[Trabalhou em dia não útil?]]="Sim",tbCalculoValeTransporte[[#This Row],[Faltou no dia?]]="Sim"),-1,IF(VLOOKUP(tbCalculoValeTransporte[[#This Row],[Dia]],tbJornada[[Abreviatura]:[É dia util?]],2,FALSE)="Sim",IF(ISERROR(VLOOKUP(TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"dd-mmm"),tbFeriados[Dia / Mês],1,FALSE)),IF(NOT(tbCalculoValeTransporte[[#This Row],[Faltou no dia?]]="Sim"),1,0),0),IF(tbCalculoValeTransporte[[#This Row],[Trabalhou em dia não útil?]]="Sim",1,0))),"")</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="H32" s="5" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[sts]]=1,TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"dd-mmm")&amp;"-"&amp;$D$3,"")</f>
-        <v>27-jan-2017</v>
+        <v/>
       </c>
       <c r="I32" s="34" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[sts]]&lt;0,"Não pode marcar como trabalhado no dia útil e faltado ao mesmo tempo","")</f>
@@ -3588,24 +3571,24 @@
       </c>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B33" s="21">
+      <c r="B33" s="21" t="str">
         <f t="shared" si="0"/>
-        <v>42763</v>
+        <v/>
       </c>
       <c r="C33" s="5" t="str">
         <f>TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"ddd")</f>
-        <v>sáb</v>
+        <v/>
       </c>
       <c r="D33" s="35"/>
       <c r="E33" s="36"/>
       <c r="F33" s="36"/>
-      <c r="G33" s="33">
+      <c r="G33" s="33" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[Data]]&lt;&gt;"",IF(AND(tbCalculoValeTransporte[[#This Row],[Trabalhou em dia não útil?]]="Sim",tbCalculoValeTransporte[[#This Row],[Faltou no dia?]]="Sim"),-1,IF(VLOOKUP(tbCalculoValeTransporte[[#This Row],[Dia]],tbJornada[[Abreviatura]:[É dia util?]],2,FALSE)="Sim",IF(ISERROR(VLOOKUP(TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"dd-mmm"),tbFeriados[Dia / Mês],1,FALSE)),IF(NOT(tbCalculoValeTransporte[[#This Row],[Faltou no dia?]]="Sim"),1,0),0),IF(tbCalculoValeTransporte[[#This Row],[Trabalhou em dia não útil?]]="Sim",1,0))),"")</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="H33" s="5" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[sts]]=1,TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"dd-mmm")&amp;"-"&amp;$D$3,"")</f>
-        <v>28-jan-2017</v>
+        <v/>
       </c>
       <c r="I33" s="34" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[sts]]&lt;0,"Não pode marcar como trabalhado no dia útil e faltado ao mesmo tempo","")</f>
@@ -3613,20 +3596,20 @@
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B34" s="21">
+      <c r="B34" s="21" t="str">
         <f t="shared" si="0"/>
-        <v>42764</v>
+        <v/>
       </c>
       <c r="C34" s="5" t="str">
         <f>TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"ddd")</f>
-        <v>dom</v>
+        <v/>
       </c>
       <c r="D34" s="35"/>
       <c r="E34" s="36"/>
       <c r="F34" s="36"/>
-      <c r="G34" s="33">
+      <c r="G34" s="33" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[Data]]&lt;&gt;"",IF(AND(tbCalculoValeTransporte[[#This Row],[Trabalhou em dia não útil?]]="Sim",tbCalculoValeTransporte[[#This Row],[Faltou no dia?]]="Sim"),-1,IF(VLOOKUP(tbCalculoValeTransporte[[#This Row],[Dia]],tbJornada[[Abreviatura]:[É dia util?]],2,FALSE)="Sim",IF(ISERROR(VLOOKUP(TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"dd-mmm"),tbFeriados[Dia / Mês],1,FALSE)),IF(NOT(tbCalculoValeTransporte[[#This Row],[Faltou no dia?]]="Sim"),1,0),0),IF(tbCalculoValeTransporte[[#This Row],[Trabalhou em dia não útil?]]="Sim",1,0))),"")</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="H34" s="5" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[sts]]=1,TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"dd-mmm")&amp;"-"&amp;$D$3,"")</f>
@@ -3638,24 +3621,24 @@
       </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B35" s="21">
+      <c r="B35" s="21" t="str">
         <f t="shared" si="0"/>
-        <v>42765</v>
+        <v/>
       </c>
       <c r="C35" s="5" t="str">
         <f>TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"ddd")</f>
-        <v>seg</v>
+        <v/>
       </c>
       <c r="D35" s="35"/>
       <c r="E35" s="36"/>
       <c r="F35" s="36"/>
-      <c r="G35" s="33">
+      <c r="G35" s="33" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[Data]]&lt;&gt;"",IF(AND(tbCalculoValeTransporte[[#This Row],[Trabalhou em dia não útil?]]="Sim",tbCalculoValeTransporte[[#This Row],[Faltou no dia?]]="Sim"),-1,IF(VLOOKUP(tbCalculoValeTransporte[[#This Row],[Dia]],tbJornada[[Abreviatura]:[É dia util?]],2,FALSE)="Sim",IF(ISERROR(VLOOKUP(TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"dd-mmm"),tbFeriados[Dia / Mês],1,FALSE)),IF(NOT(tbCalculoValeTransporte[[#This Row],[Faltou no dia?]]="Sim"),1,0),0),IF(tbCalculoValeTransporte[[#This Row],[Trabalhou em dia não útil?]]="Sim",1,0))),"")</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="H35" s="5" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[sts]]=1,TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"dd-mmm")&amp;"-"&amp;$D$3,"")</f>
-        <v>30-jan-2017</v>
+        <v/>
       </c>
       <c r="I35" s="34" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[sts]]&lt;0,"Não pode marcar como trabalhado no dia útil e faltado ao mesmo tempo","")</f>
@@ -3663,24 +3646,24 @@
       </c>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B36" s="21">
+      <c r="B36" s="21" t="str">
         <f t="shared" si="0"/>
-        <v>42766</v>
+        <v/>
       </c>
       <c r="C36" s="5" t="str">
         <f>TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"ddd")</f>
-        <v>ter</v>
+        <v/>
       </c>
       <c r="D36" s="35"/>
       <c r="E36" s="36"/>
       <c r="F36" s="36"/>
-      <c r="G36" s="33">
+      <c r="G36" s="33" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[Data]]&lt;&gt;"",IF(AND(tbCalculoValeTransporte[[#This Row],[Trabalhou em dia não útil?]]="Sim",tbCalculoValeTransporte[[#This Row],[Faltou no dia?]]="Sim"),-1,IF(VLOOKUP(tbCalculoValeTransporte[[#This Row],[Dia]],tbJornada[[Abreviatura]:[É dia util?]],2,FALSE)="Sim",IF(ISERROR(VLOOKUP(TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"dd-mmm"),tbFeriados[Dia / Mês],1,FALSE)),IF(NOT(tbCalculoValeTransporte[[#This Row],[Faltou no dia?]]="Sim"),1,0),0),IF(tbCalculoValeTransporte[[#This Row],[Trabalhou em dia não útil?]]="Sim",1,0))),"")</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="H36" s="5" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[sts]]=1,TEXT(tbCalculoValeTransporte[[#This Row],[Data]],"dd-mmm")&amp;"-"&amp;$D$3,"")</f>
-        <v>31-jan-2017</v>
+        <v/>
       </c>
       <c r="I36" s="34" t="str">
         <f>IF(tbCalculoValeTransporte[[#This Row],[sts]]&lt;0,"Não pode marcar como trabalhado no dia útil e faltado ao mesmo tempo","")</f>
@@ -3768,7 +3751,7 @@
       <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="E9" sqref="E9:F9"/>
+      <selection pane="bottomRight" activeCell="E13" sqref="E13:M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15.75" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -3778,7 +3761,7 @@
     <col min="4" max="4" width="20.7109375" style="40" customWidth="1"/>
     <col min="5" max="13" width="9.140625" style="4" customWidth="1"/>
     <col min="14" max="14" width="2.7109375" style="4" customWidth="1"/>
-    <col min="15" max="17" width="0" style="4" hidden="1"/>
+    <col min="15" max="17" width="0" style="4" hidden="1" customWidth="1"/>
     <col min="18" max="16384" width="9.140625" style="4" hidden="1"/>
   </cols>
   <sheetData>
@@ -3786,46 +3769,46 @@
       <c r="A1" s="39" t="s">
         <v>83</v>
       </c>
-      <c r="D1" s="68" t="s">
+      <c r="D1" s="95" t="s">
         <v>89</v>
       </c>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
+      <c r="E1" s="95"/>
+      <c r="F1" s="95"/>
+      <c r="G1" s="95"/>
+      <c r="H1" s="95"/>
+      <c r="I1" s="95"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D2" s="69" t="s">
+      <c r="D2" s="96" t="s">
         <v>103</v>
       </c>
-      <c r="E2" s="69"/>
-      <c r="F2" s="65" t="s">
+      <c r="E2" s="96"/>
+      <c r="F2" s="92" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="66"/>
-      <c r="H2" s="66"/>
-      <c r="I2" s="67"/>
+      <c r="G2" s="93"/>
+      <c r="H2" s="93"/>
+      <c r="I2" s="94"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D3" s="69" t="s">
+      <c r="D3" s="96" t="s">
         <v>87</v>
       </c>
-      <c r="E3" s="69"/>
-      <c r="F3" s="65" t="s">
+      <c r="E3" s="96"/>
+      <c r="F3" s="92" t="s">
         <v>90</v>
       </c>
-      <c r="G3" s="66"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="67"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="93"/>
+      <c r="I3" s="94"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D4" s="69" t="s">
+      <c r="D4" s="96" t="s">
         <v>88</v>
       </c>
-      <c r="E4" s="70"/>
-      <c r="F4" s="65"/>
-      <c r="G4" s="67"/>
+      <c r="E4" s="97"/>
+      <c r="F4" s="92"/>
+      <c r="G4" s="94"/>
       <c r="H4" s="42"/>
       <c r="I4" s="42"/>
     </row>
@@ -3837,166 +3820,166 @@
       <c r="I5" s="41"/>
     </row>
     <row r="6" spans="1:14" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="71"/>
-      <c r="D6" s="72"/>
-      <c r="E6" s="72"/>
-      <c r="F6" s="73"/>
-      <c r="G6" s="73"/>
-      <c r="H6" s="74"/>
-      <c r="I6" s="74"/>
-      <c r="J6" s="75"/>
-      <c r="K6" s="75"/>
-      <c r="L6" s="75"/>
-      <c r="M6" s="75"/>
-      <c r="N6" s="76"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="48"/>
+      <c r="G6" s="48"/>
+      <c r="H6" s="49"/>
+      <c r="I6" s="49"/>
+      <c r="J6" s="50"/>
+      <c r="K6" s="50"/>
+      <c r="L6" s="50"/>
+      <c r="M6" s="50"/>
+      <c r="N6" s="51"/>
     </row>
     <row r="7" spans="1:14" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="C7" s="77"/>
-      <c r="D7" s="78" t="s">
+      <c r="C7" s="52"/>
+      <c r="D7" s="85" t="s">
         <v>84</v>
       </c>
-      <c r="E7" s="78"/>
-      <c r="F7" s="78"/>
-      <c r="G7" s="78"/>
-      <c r="H7" s="78"/>
-      <c r="I7" s="78"/>
-      <c r="J7" s="78"/>
-      <c r="K7" s="78"/>
-      <c r="L7" s="78"/>
-      <c r="M7" s="78"/>
-      <c r="N7" s="79"/>
+      <c r="E7" s="85"/>
+      <c r="F7" s="85"/>
+      <c r="G7" s="85"/>
+      <c r="H7" s="85"/>
+      <c r="I7" s="85"/>
+      <c r="J7" s="85"/>
+      <c r="K7" s="85"/>
+      <c r="L7" s="85"/>
+      <c r="M7" s="85"/>
+      <c r="N7" s="53"/>
     </row>
     <row r="8" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C8" s="77"/>
-      <c r="D8" s="80"/>
-      <c r="E8" s="81"/>
-      <c r="F8" s="81"/>
-      <c r="G8" s="81"/>
-      <c r="H8" s="81"/>
-      <c r="I8" s="81"/>
-      <c r="J8" s="81"/>
-      <c r="K8" s="81"/>
-      <c r="L8" s="81"/>
-      <c r="M8" s="81"/>
-      <c r="N8" s="79"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="54"/>
+      <c r="E8" s="55"/>
+      <c r="F8" s="55"/>
+      <c r="G8" s="55"/>
+      <c r="H8" s="55"/>
+      <c r="I8" s="55"/>
+      <c r="J8" s="55"/>
+      <c r="K8" s="55"/>
+      <c r="L8" s="55"/>
+      <c r="M8" s="55"/>
+      <c r="N8" s="53"/>
     </row>
     <row r="9" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C9" s="77"/>
+      <c r="C9" s="52"/>
       <c r="D9" s="43" t="s">
         <v>85</v>
       </c>
-      <c r="E9" s="56" t="str">
+      <c r="E9" s="86" t="str">
         <f>IF(F4&lt;&gt;"",F4,"VT-"&amp;'Cálculo do Vale Transporte'!$F$3)</f>
-        <v>VT-42736</v>
-      </c>
-      <c r="F9" s="57"/>
-      <c r="G9" s="81"/>
-      <c r="H9" s="81"/>
-      <c r="I9" s="81"/>
-      <c r="J9" s="52" t="s">
+        <v>VT-</v>
+      </c>
+      <c r="F9" s="87"/>
+      <c r="G9" s="55"/>
+      <c r="H9" s="55"/>
+      <c r="I9" s="55"/>
+      <c r="J9" s="88" t="s">
         <v>86</v>
       </c>
-      <c r="K9" s="53"/>
-      <c r="L9" s="54">
+      <c r="K9" s="89"/>
+      <c r="L9" s="90">
         <f>VALOR_VALETRANSPORTE*QTD_VALETRANSPORTE*SUM(tbCalculoValeTransporte[sts])+SUM(tbCalculoValeTransporte[Custo Extra?])</f>
-        <v>301.59999999999997</v>
-      </c>
-      <c r="M9" s="55"/>
-      <c r="N9" s="79"/>
+        <v>0</v>
+      </c>
+      <c r="M9" s="91"/>
+      <c r="N9" s="53"/>
     </row>
     <row r="10" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C10" s="77"/>
-      <c r="D10" s="80"/>
-      <c r="E10" s="81"/>
-      <c r="F10" s="81"/>
-      <c r="G10" s="81"/>
-      <c r="H10" s="81"/>
-      <c r="I10" s="81"/>
-      <c r="J10" s="81"/>
-      <c r="K10" s="81"/>
-      <c r="L10" s="81"/>
-      <c r="M10" s="81"/>
-      <c r="N10" s="79"/>
+      <c r="C10" s="52"/>
+      <c r="D10" s="54"/>
+      <c r="E10" s="55"/>
+      <c r="F10" s="55"/>
+      <c r="G10" s="55"/>
+      <c r="H10" s="55"/>
+      <c r="I10" s="55"/>
+      <c r="J10" s="55"/>
+      <c r="K10" s="55"/>
+      <c r="L10" s="55"/>
+      <c r="M10" s="55"/>
+      <c r="N10" s="53"/>
     </row>
     <row r="11" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C11" s="77"/>
+      <c r="C11" s="52"/>
       <c r="D11" s="43" t="s">
         <v>81</v>
       </c>
-      <c r="E11" s="58" t="str">
+      <c r="E11" s="80" t="str">
         <f>F2</f>
         <v>John Green</v>
       </c>
-      <c r="F11" s="59"/>
-      <c r="G11" s="59"/>
-      <c r="H11" s="59"/>
-      <c r="I11" s="59"/>
-      <c r="J11" s="59"/>
-      <c r="K11" s="59"/>
-      <c r="L11" s="59"/>
-      <c r="M11" s="60"/>
-      <c r="N11" s="79"/>
+      <c r="F11" s="81"/>
+      <c r="G11" s="81"/>
+      <c r="H11" s="81"/>
+      <c r="I11" s="81"/>
+      <c r="J11" s="81"/>
+      <c r="K11" s="81"/>
+      <c r="L11" s="81"/>
+      <c r="M11" s="82"/>
+      <c r="N11" s="53"/>
     </row>
     <row r="12" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C12" s="77"/>
+      <c r="C12" s="52"/>
       <c r="D12" s="43" t="s">
         <v>94</v>
       </c>
-      <c r="E12" s="61" t="str">
+      <c r="E12" s="83" t="str">
         <f>VLOOKUP(E11,tbCadEmpregador[[Nome]:[Endereço Completo]],3,FALSE)</f>
         <v>Endereço Empregador aqui!</v>
       </c>
-      <c r="F12" s="61"/>
-      <c r="G12" s="61"/>
-      <c r="H12" s="61"/>
-      <c r="I12" s="61"/>
-      <c r="J12" s="61"/>
-      <c r="K12" s="61"/>
-      <c r="L12" s="61"/>
-      <c r="M12" s="61"/>
-      <c r="N12" s="79"/>
+      <c r="F12" s="83"/>
+      <c r="G12" s="83"/>
+      <c r="H12" s="83"/>
+      <c r="I12" s="83"/>
+      <c r="J12" s="83"/>
+      <c r="K12" s="83"/>
+      <c r="L12" s="83"/>
+      <c r="M12" s="83"/>
+      <c r="N12" s="53"/>
     </row>
     <row r="13" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C13" s="77"/>
+      <c r="C13" s="52"/>
       <c r="D13" s="43" t="s">
         <v>93</v>
       </c>
-      <c r="E13" s="58" t="str">
+      <c r="E13" s="80" t="str">
         <f>[1]!VALOREXTENSO(L9)</f>
-        <v>trezentos e um reais e sessenta centavos</v>
-      </c>
-      <c r="F13" s="59"/>
-      <c r="G13" s="59"/>
-      <c r="H13" s="59"/>
-      <c r="I13" s="59"/>
-      <c r="J13" s="59"/>
-      <c r="K13" s="59"/>
-      <c r="L13" s="59"/>
-      <c r="M13" s="60"/>
-      <c r="N13" s="79"/>
+        <v/>
+      </c>
+      <c r="F13" s="81"/>
+      <c r="G13" s="81"/>
+      <c r="H13" s="81"/>
+      <c r="I13" s="81"/>
+      <c r="J13" s="81"/>
+      <c r="K13" s="81"/>
+      <c r="L13" s="81"/>
+      <c r="M13" s="82"/>
+      <c r="N13" s="53"/>
     </row>
     <row r="14" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C14" s="77"/>
+      <c r="C14" s="52"/>
       <c r="D14" s="43" t="s">
         <v>95</v>
       </c>
-      <c r="E14" s="61" t="str">
+      <c r="E14" s="83" t="str">
         <f>"Vale Transporte do mês de "&amp;'Cálculo do Vale Transporte'!B3&amp;" de "&amp;'Cálculo do Vale Transporte'!D3&amp;". Comtenplando os dias abaixo:"</f>
-        <v>Vale Transporte do mês de Janeiro de 2017. Comtenplando os dias abaixo:</v>
-      </c>
-      <c r="F14" s="61"/>
-      <c r="G14" s="61"/>
-      <c r="H14" s="61"/>
-      <c r="I14" s="61"/>
-      <c r="J14" s="61"/>
-      <c r="K14" s="61"/>
-      <c r="L14" s="61"/>
-      <c r="M14" s="61"/>
-      <c r="N14" s="79"/>
+        <v>Vale Transporte do mês de  de . Comtenplando os dias abaixo:</v>
+      </c>
+      <c r="F14" s="83"/>
+      <c r="G14" s="83"/>
+      <c r="H14" s="83"/>
+      <c r="I14" s="83"/>
+      <c r="J14" s="83"/>
+      <c r="K14" s="83"/>
+      <c r="L14" s="83"/>
+      <c r="M14" s="83"/>
+      <c r="N14" s="53"/>
     </row>
     <row r="15" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C15" s="77"/>
-      <c r="D15" s="62" t="str">
+      <c r="C15" s="52"/>
+      <c r="D15" s="77" t="str">
         <f>"==="
 &amp;IF('Cálculo do Vale Transporte'!H6&lt;&gt;"",'Cálculo do Vale Transporte'!H6,"")
 &amp;IF('Cálculo do Vale Transporte'!H7&lt;&gt;""," / "&amp;'Cálculo do Vale Transporte'!H7,"")
@@ -4006,22 +3989,22 @@
 &amp;IF('Cálculo do Vale Transporte'!H11&lt;&gt;""," / "&amp;'Cálculo do Vale Transporte'!H11,"")
 &amp;IF('Cálculo do Vale Transporte'!H12&lt;&gt;""," / "&amp;'Cálculo do Vale Transporte'!H12,"")
 &amp;"==="</f>
-        <v>=== / 02-jan-2017 / 03-jan-2017 / 04-jan-2017 / 05-jan-2017 / 06-jan-2017 / 07-jan-2017===</v>
-      </c>
-      <c r="E15" s="63"/>
-      <c r="F15" s="63"/>
-      <c r="G15" s="63"/>
-      <c r="H15" s="63"/>
-      <c r="I15" s="63"/>
-      <c r="J15" s="63"/>
-      <c r="K15" s="63"/>
-      <c r="L15" s="63"/>
-      <c r="M15" s="64"/>
-      <c r="N15" s="79"/>
+        <v>======</v>
+      </c>
+      <c r="E15" s="78"/>
+      <c r="F15" s="78"/>
+      <c r="G15" s="78"/>
+      <c r="H15" s="78"/>
+      <c r="I15" s="78"/>
+      <c r="J15" s="78"/>
+      <c r="K15" s="78"/>
+      <c r="L15" s="78"/>
+      <c r="M15" s="79"/>
+      <c r="N15" s="53"/>
     </row>
     <row r="16" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C16" s="77"/>
-      <c r="D16" s="62" t="str">
+      <c r="C16" s="52"/>
+      <c r="D16" s="77" t="str">
         <f>"===="
 &amp;IF('Cálculo do Vale Transporte'!H13&lt;&gt;""," / "&amp;'Cálculo do Vale Transporte'!H13,"")
 &amp;IF('Cálculo do Vale Transporte'!H14&lt;&gt;""," / "&amp;'Cálculo do Vale Transporte'!H14,"")
@@ -4031,22 +4014,22 @@
 &amp;IF('Cálculo do Vale Transporte'!H18&lt;&gt;""," / "&amp;'Cálculo do Vale Transporte'!H18,"")
 &amp;IF('Cálculo do Vale Transporte'!H19&lt;&gt;""," / "&amp;'Cálculo do Vale Transporte'!H19,"")
 &amp;"==="</f>
-        <v>==== / 09-jan-2017 / 10-jan-2017 / 11-jan-2017 / 12-jan-2017 / 13-jan-2017 / 14-jan-2017===</v>
-      </c>
-      <c r="E16" s="63"/>
-      <c r="F16" s="63"/>
-      <c r="G16" s="63"/>
-      <c r="H16" s="63"/>
-      <c r="I16" s="63"/>
-      <c r="J16" s="63"/>
-      <c r="K16" s="63"/>
-      <c r="L16" s="63"/>
-      <c r="M16" s="64"/>
-      <c r="N16" s="79"/>
+        <v>=======</v>
+      </c>
+      <c r="E16" s="78"/>
+      <c r="F16" s="78"/>
+      <c r="G16" s="78"/>
+      <c r="H16" s="78"/>
+      <c r="I16" s="78"/>
+      <c r="J16" s="78"/>
+      <c r="K16" s="78"/>
+      <c r="L16" s="78"/>
+      <c r="M16" s="79"/>
+      <c r="N16" s="53"/>
     </row>
     <row r="17" spans="3:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C17" s="77"/>
-      <c r="D17" s="62" t="str">
+      <c r="C17" s="52"/>
+      <c r="D17" s="77" t="str">
         <f>"==="
 &amp;IF('Cálculo do Vale Transporte'!H20&lt;&gt;""," / "&amp;'Cálculo do Vale Transporte'!H20,"")
 &amp;IF('Cálculo do Vale Transporte'!H21&lt;&gt;""," / "&amp;'Cálculo do Vale Transporte'!H21,"")
@@ -4056,22 +4039,22 @@
 &amp;IF('Cálculo do Vale Transporte'!H25&lt;&gt;""," / "&amp;'Cálculo do Vale Transporte'!H25,"")
 &amp;IF('Cálculo do Vale Transporte'!H26&lt;&gt;""," / "&amp;'Cálculo do Vale Transporte'!H26,"")
 &amp;"==="</f>
-        <v>=== / 16-jan-2017 / 17-jan-2017 / 18-jan-2017 / 19-jan-2017 / 20-jan-2017 / 21-jan-2017===</v>
-      </c>
-      <c r="E17" s="63"/>
-      <c r="F17" s="63"/>
-      <c r="G17" s="63"/>
-      <c r="H17" s="63"/>
-      <c r="I17" s="63"/>
-      <c r="J17" s="63"/>
-      <c r="K17" s="63"/>
-      <c r="L17" s="63"/>
-      <c r="M17" s="64"/>
-      <c r="N17" s="79"/>
+        <v>======</v>
+      </c>
+      <c r="E17" s="78"/>
+      <c r="F17" s="78"/>
+      <c r="G17" s="78"/>
+      <c r="H17" s="78"/>
+      <c r="I17" s="78"/>
+      <c r="J17" s="78"/>
+      <c r="K17" s="78"/>
+      <c r="L17" s="78"/>
+      <c r="M17" s="79"/>
+      <c r="N17" s="53"/>
     </row>
     <row r="18" spans="3:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C18" s="77"/>
-      <c r="D18" s="62" t="str">
+      <c r="C18" s="52"/>
+      <c r="D18" s="77" t="str">
         <f>"==="
 &amp;IF('Cálculo do Vale Transporte'!H27&lt;&gt;"",'Cálculo do Vale Transporte'!H27,"")
 &amp;IF('Cálculo do Vale Transporte'!H28&lt;&gt;"","/"&amp;'Cálculo do Vale Transporte'!H28,"")
@@ -4081,528 +4064,542 @@
 &amp;IF('Cálculo do Vale Transporte'!H32&lt;&gt;"","/"&amp;'Cálculo do Vale Transporte'!H32,"")
 &amp;IF('Cálculo do Vale Transporte'!H33&lt;&gt;"","/"&amp;'Cálculo do Vale Transporte'!H33,"")
 &amp;"==="</f>
-        <v>===/23-jan-2017/24-jan-2017/25-jan-2017/26-jan-2017/27-jan-2017/28-jan-2017===</v>
-      </c>
-      <c r="E18" s="63"/>
-      <c r="F18" s="63"/>
-      <c r="G18" s="63"/>
-      <c r="H18" s="63"/>
-      <c r="I18" s="63"/>
-      <c r="J18" s="63"/>
-      <c r="K18" s="63"/>
-      <c r="L18" s="63"/>
-      <c r="M18" s="64"/>
-      <c r="N18" s="79"/>
+        <v>======</v>
+      </c>
+      <c r="E18" s="78"/>
+      <c r="F18" s="78"/>
+      <c r="G18" s="78"/>
+      <c r="H18" s="78"/>
+      <c r="I18" s="78"/>
+      <c r="J18" s="78"/>
+      <c r="K18" s="78"/>
+      <c r="L18" s="78"/>
+      <c r="M18" s="79"/>
+      <c r="N18" s="53"/>
     </row>
     <row r="19" spans="3:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C19" s="77"/>
-      <c r="D19" s="62" t="str">
+      <c r="C19" s="52"/>
+      <c r="D19" s="77" t="str">
         <f>"==="
 &amp;IF('Cálculo do Vale Transporte'!H34&lt;&gt;"","/"&amp;'Cálculo do Vale Transporte'!H34,"")
 &amp;IF('Cálculo do Vale Transporte'!H35&lt;&gt;"","/"&amp;'Cálculo do Vale Transporte'!H35,"")
 &amp;IF('Cálculo do Vale Transporte'!H36&lt;&gt;"","/"&amp;'Cálculo do Vale Transporte'!H36,"")
 &amp;"==="</f>
-        <v>===/30-jan-2017/31-jan-2017===</v>
-      </c>
-      <c r="E19" s="63"/>
-      <c r="F19" s="63"/>
-      <c r="G19" s="63"/>
-      <c r="H19" s="63"/>
-      <c r="I19" s="63"/>
-      <c r="J19" s="63"/>
-      <c r="K19" s="63"/>
-      <c r="L19" s="63"/>
-      <c r="M19" s="64"/>
-      <c r="N19" s="79"/>
+        <v>======</v>
+      </c>
+      <c r="E19" s="78"/>
+      <c r="F19" s="78"/>
+      <c r="G19" s="78"/>
+      <c r="H19" s="78"/>
+      <c r="I19" s="78"/>
+      <c r="J19" s="78"/>
+      <c r="K19" s="78"/>
+      <c r="L19" s="78"/>
+      <c r="M19" s="79"/>
+      <c r="N19" s="53"/>
     </row>
     <row r="20" spans="3:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C20" s="77"/>
-      <c r="D20" s="80"/>
-      <c r="E20" s="81"/>
-      <c r="F20" s="81"/>
-      <c r="G20" s="81"/>
-      <c r="H20" s="81"/>
-      <c r="I20" s="81"/>
-      <c r="J20" s="81"/>
-      <c r="K20" s="81"/>
-      <c r="L20" s="81"/>
-      <c r="M20" s="81"/>
-      <c r="N20" s="79"/>
+      <c r="C20" s="52"/>
+      <c r="D20" s="54"/>
+      <c r="E20" s="55"/>
+      <c r="F20" s="55"/>
+      <c r="G20" s="55"/>
+      <c r="H20" s="55"/>
+      <c r="I20" s="55"/>
+      <c r="J20" s="55"/>
+      <c r="K20" s="55"/>
+      <c r="L20" s="55"/>
+      <c r="M20" s="55"/>
+      <c r="N20" s="53"/>
     </row>
     <row r="21" spans="3:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C21" s="77"/>
-      <c r="D21" s="82" t="str">
+      <c r="C21" s="52"/>
+      <c r="D21" s="56" t="str">
         <f ca="1">tbCadEmpregador[Cidade (Recibo)]&amp;", "&amp;TEXT(NOW(),"dd")&amp;" de "&amp;TEXT(NOW(),"mmmm")&amp;" de "&amp;TEXT(NOW(),"aaaa"&amp;".")</f>
-        <v>Brasília, 06 de janeiro de 2017.</v>
-      </c>
-      <c r="E21" s="81"/>
-      <c r="F21" s="81"/>
-      <c r="G21" s="81"/>
-      <c r="H21" s="81"/>
-      <c r="I21" s="81"/>
-      <c r="J21" s="81"/>
-      <c r="K21" s="81"/>
-      <c r="L21" s="81"/>
-      <c r="M21" s="81"/>
-      <c r="N21" s="79"/>
+        <v>Brasília, 24 de fevereiro de 2017.</v>
+      </c>
+      <c r="E21" s="55"/>
+      <c r="F21" s="55"/>
+      <c r="G21" s="55"/>
+      <c r="H21" s="55"/>
+      <c r="I21" s="55"/>
+      <c r="J21" s="55"/>
+      <c r="K21" s="55"/>
+      <c r="L21" s="55"/>
+      <c r="M21" s="55"/>
+      <c r="N21" s="53"/>
     </row>
     <row r="22" spans="3:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C22" s="77"/>
-      <c r="D22" s="80"/>
-      <c r="E22" s="81"/>
-      <c r="F22" s="81"/>
-      <c r="G22" s="81"/>
-      <c r="H22" s="81"/>
-      <c r="I22" s="81"/>
-      <c r="J22" s="81"/>
-      <c r="K22" s="81"/>
-      <c r="L22" s="81"/>
-      <c r="M22" s="81"/>
-      <c r="N22" s="79"/>
+      <c r="C22" s="52"/>
+      <c r="D22" s="54"/>
+      <c r="E22" s="55"/>
+      <c r="F22" s="55"/>
+      <c r="G22" s="55"/>
+      <c r="H22" s="55"/>
+      <c r="I22" s="55"/>
+      <c r="J22" s="55"/>
+      <c r="K22" s="55"/>
+      <c r="L22" s="55"/>
+      <c r="M22" s="55"/>
+      <c r="N22" s="53"/>
       <c r="P22" s="22"/>
     </row>
     <row r="23" spans="3:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C23" s="77"/>
+      <c r="C23" s="52"/>
       <c r="D23" s="43" t="s">
         <v>100</v>
       </c>
-      <c r="E23" s="58" t="str">
+      <c r="E23" s="80" t="str">
         <f>F3</f>
         <v>Mary Green</v>
       </c>
-      <c r="F23" s="59"/>
-      <c r="G23" s="59"/>
-      <c r="H23" s="59"/>
-      <c r="I23" s="60"/>
+      <c r="F23" s="81"/>
+      <c r="G23" s="81"/>
+      <c r="H23" s="81"/>
+      <c r="I23" s="82"/>
       <c r="J23" s="43" t="s">
         <v>101</v>
       </c>
-      <c r="K23" s="59" t="str">
+      <c r="K23" s="81" t="str">
         <f>VLOOKUP(E23,tbCadDomestico[[Nome]:[CPF]],2,FALSE)</f>
         <v>123.456.789-99</v>
       </c>
-      <c r="L23" s="59"/>
-      <c r="M23" s="60"/>
-      <c r="N23" s="79"/>
+      <c r="L23" s="81"/>
+      <c r="M23" s="82"/>
+      <c r="N23" s="53"/>
     </row>
     <row r="24" spans="3:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C24" s="77"/>
+      <c r="C24" s="52"/>
       <c r="D24" s="43" t="s">
         <v>94</v>
       </c>
-      <c r="E24" s="61" t="str">
+      <c r="E24" s="83" t="str">
         <f>VLOOKUP(E23,tbCadDomestico[[Nome]:[Endereço Completo]],3,FALSE)</f>
         <v>Rua xyz, Qd. Z, Lt. Y, Setor Rincon Park Ceul Brasília -DF</v>
       </c>
-      <c r="F24" s="61"/>
-      <c r="G24" s="61"/>
-      <c r="H24" s="61"/>
-      <c r="I24" s="61"/>
-      <c r="J24" s="61"/>
-      <c r="K24" s="61"/>
-      <c r="L24" s="61"/>
-      <c r="M24" s="61"/>
-      <c r="N24" s="79"/>
+      <c r="F24" s="83"/>
+      <c r="G24" s="83"/>
+      <c r="H24" s="83"/>
+      <c r="I24" s="83"/>
+      <c r="J24" s="83"/>
+      <c r="K24" s="83"/>
+      <c r="L24" s="83"/>
+      <c r="M24" s="83"/>
+      <c r="N24" s="53"/>
     </row>
     <row r="25" spans="3:16" s="45" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="C25" s="83"/>
+      <c r="C25" s="57"/>
       <c r="D25" s="44" t="s">
         <v>102</v>
       </c>
-      <c r="E25" s="51"/>
-      <c r="F25" s="51"/>
-      <c r="G25" s="51"/>
-      <c r="H25" s="51"/>
-      <c r="I25" s="51"/>
-      <c r="J25" s="51"/>
-      <c r="K25" s="51"/>
-      <c r="L25" s="51"/>
-      <c r="M25" s="51"/>
-      <c r="N25" s="84"/>
+      <c r="E25" s="84"/>
+      <c r="F25" s="84"/>
+      <c r="G25" s="84"/>
+      <c r="H25" s="84"/>
+      <c r="I25" s="84"/>
+      <c r="J25" s="84"/>
+      <c r="K25" s="84"/>
+      <c r="L25" s="84"/>
+      <c r="M25" s="84"/>
+      <c r="N25" s="58"/>
     </row>
     <row r="26" spans="3:16" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C26" s="85"/>
-      <c r="D26" s="86"/>
-      <c r="E26" s="87"/>
-      <c r="F26" s="87"/>
-      <c r="G26" s="87"/>
-      <c r="H26" s="87"/>
-      <c r="I26" s="87"/>
-      <c r="J26" s="87"/>
-      <c r="K26" s="87"/>
-      <c r="L26" s="87"/>
-      <c r="M26" s="87"/>
-      <c r="N26" s="88"/>
+      <c r="C26" s="59"/>
+      <c r="D26" s="60"/>
+      <c r="E26" s="61"/>
+      <c r="F26" s="61"/>
+      <c r="G26" s="61"/>
+      <c r="H26" s="61"/>
+      <c r="I26" s="61"/>
+      <c r="J26" s="61"/>
+      <c r="K26" s="61"/>
+      <c r="L26" s="61"/>
+      <c r="M26" s="61"/>
+      <c r="N26" s="62"/>
     </row>
     <row r="27" spans="3:16" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C27" s="89"/>
-      <c r="D27" s="90"/>
-      <c r="E27" s="91"/>
-      <c r="F27" s="91"/>
-      <c r="G27" s="91"/>
-      <c r="H27" s="91"/>
-      <c r="I27" s="91"/>
-      <c r="J27" s="91"/>
-      <c r="K27" s="91"/>
-      <c r="L27" s="91"/>
-      <c r="M27" s="91"/>
-      <c r="N27" s="92"/>
+      <c r="C27" s="63"/>
+      <c r="D27" s="64"/>
+      <c r="E27" s="65"/>
+      <c r="F27" s="65"/>
+      <c r="G27" s="65"/>
+      <c r="H27" s="65"/>
+      <c r="I27" s="65"/>
+      <c r="J27" s="65"/>
+      <c r="K27" s="65"/>
+      <c r="L27" s="65"/>
+      <c r="M27" s="65"/>
+      <c r="N27" s="66"/>
     </row>
     <row r="28" spans="3:16" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="C28" s="77"/>
-      <c r="D28" s="78" t="str">
+      <c r="C28" s="52"/>
+      <c r="D28" s="85" t="str">
         <f>D7</f>
         <v>Recibo</v>
       </c>
-      <c r="E28" s="78"/>
-      <c r="F28" s="78"/>
-      <c r="G28" s="78"/>
-      <c r="H28" s="78"/>
-      <c r="I28" s="78"/>
-      <c r="J28" s="78"/>
-      <c r="K28" s="78"/>
-      <c r="L28" s="78"/>
-      <c r="M28" s="78"/>
-      <c r="N28" s="79"/>
+      <c r="E28" s="85"/>
+      <c r="F28" s="85"/>
+      <c r="G28" s="85"/>
+      <c r="H28" s="85"/>
+      <c r="I28" s="85"/>
+      <c r="J28" s="85"/>
+      <c r="K28" s="85"/>
+      <c r="L28" s="85"/>
+      <c r="M28" s="85"/>
+      <c r="N28" s="53"/>
     </row>
     <row r="29" spans="3:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C29" s="77"/>
-      <c r="D29" s="80"/>
-      <c r="E29" s="81"/>
-      <c r="F29" s="81"/>
-      <c r="G29" s="81"/>
-      <c r="H29" s="81"/>
-      <c r="I29" s="81"/>
-      <c r="J29" s="81"/>
-      <c r="K29" s="81"/>
-      <c r="L29" s="81"/>
-      <c r="M29" s="81"/>
-      <c r="N29" s="79"/>
+      <c r="C29" s="52"/>
+      <c r="D29" s="54"/>
+      <c r="E29" s="55"/>
+      <c r="F29" s="55"/>
+      <c r="G29" s="55"/>
+      <c r="H29" s="55"/>
+      <c r="I29" s="55"/>
+      <c r="J29" s="55"/>
+      <c r="K29" s="55"/>
+      <c r="L29" s="55"/>
+      <c r="M29" s="55"/>
+      <c r="N29" s="53"/>
     </row>
     <row r="30" spans="3:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C30" s="77"/>
+      <c r="C30" s="52"/>
       <c r="D30" s="43" t="s">
         <v>85</v>
       </c>
-      <c r="E30" s="56" t="str">
+      <c r="E30" s="86" t="str">
         <f>E9</f>
-        <v>VT-42736</v>
-      </c>
-      <c r="F30" s="57"/>
-      <c r="G30" s="81"/>
-      <c r="H30" s="81"/>
-      <c r="I30" s="81"/>
-      <c r="J30" s="52" t="s">
+        <v>VT-</v>
+      </c>
+      <c r="F30" s="87"/>
+      <c r="G30" s="55"/>
+      <c r="H30" s="55"/>
+      <c r="I30" s="55"/>
+      <c r="J30" s="88" t="s">
         <v>86</v>
       </c>
-      <c r="K30" s="53"/>
-      <c r="L30" s="54">
+      <c r="K30" s="89"/>
+      <c r="L30" s="90">
         <f>L9</f>
-        <v>301.59999999999997</v>
-      </c>
-      <c r="M30" s="55"/>
-      <c r="N30" s="79"/>
+        <v>0</v>
+      </c>
+      <c r="M30" s="91"/>
+      <c r="N30" s="53"/>
     </row>
     <row r="31" spans="3:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C31" s="77"/>
-      <c r="D31" s="80"/>
-      <c r="E31" s="81"/>
-      <c r="F31" s="81"/>
-      <c r="G31" s="81"/>
-      <c r="H31" s="81"/>
-      <c r="I31" s="81"/>
-      <c r="J31" s="81"/>
-      <c r="K31" s="81"/>
-      <c r="L31" s="81"/>
-      <c r="M31" s="81"/>
-      <c r="N31" s="79"/>
+      <c r="C31" s="52"/>
+      <c r="D31" s="54"/>
+      <c r="E31" s="55"/>
+      <c r="F31" s="55"/>
+      <c r="G31" s="55"/>
+      <c r="H31" s="55"/>
+      <c r="I31" s="55"/>
+      <c r="J31" s="55"/>
+      <c r="K31" s="55"/>
+      <c r="L31" s="55"/>
+      <c r="M31" s="55"/>
+      <c r="N31" s="53"/>
     </row>
     <row r="32" spans="3:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C32" s="77"/>
+      <c r="C32" s="52"/>
       <c r="D32" s="43" t="s">
         <v>81</v>
       </c>
-      <c r="E32" s="58" t="str">
+      <c r="E32" s="80" t="str">
         <f>E11</f>
         <v>John Green</v>
       </c>
-      <c r="F32" s="59"/>
-      <c r="G32" s="59"/>
-      <c r="H32" s="59"/>
-      <c r="I32" s="59"/>
-      <c r="J32" s="59"/>
-      <c r="K32" s="59"/>
-      <c r="L32" s="59"/>
-      <c r="M32" s="60"/>
-      <c r="N32" s="79"/>
+      <c r="F32" s="81"/>
+      <c r="G32" s="81"/>
+      <c r="H32" s="81"/>
+      <c r="I32" s="81"/>
+      <c r="J32" s="81"/>
+      <c r="K32" s="81"/>
+      <c r="L32" s="81"/>
+      <c r="M32" s="82"/>
+      <c r="N32" s="53"/>
     </row>
     <row r="33" spans="3:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C33" s="77"/>
+      <c r="C33" s="52"/>
       <c r="D33" s="43" t="s">
         <v>94</v>
       </c>
-      <c r="E33" s="61" t="str">
+      <c r="E33" s="83" t="str">
         <f>E12</f>
         <v>Endereço Empregador aqui!</v>
       </c>
-      <c r="F33" s="61"/>
-      <c r="G33" s="61"/>
-      <c r="H33" s="61"/>
-      <c r="I33" s="61"/>
-      <c r="J33" s="61"/>
-      <c r="K33" s="61"/>
-      <c r="L33" s="61"/>
-      <c r="M33" s="61"/>
-      <c r="N33" s="79"/>
+      <c r="F33" s="83"/>
+      <c r="G33" s="83"/>
+      <c r="H33" s="83"/>
+      <c r="I33" s="83"/>
+      <c r="J33" s="83"/>
+      <c r="K33" s="83"/>
+      <c r="L33" s="83"/>
+      <c r="M33" s="83"/>
+      <c r="N33" s="53"/>
     </row>
     <row r="34" spans="3:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C34" s="77"/>
+      <c r="C34" s="52"/>
       <c r="D34" s="43" t="s">
         <v>93</v>
       </c>
-      <c r="E34" s="58" t="str">
+      <c r="E34" s="80" t="str">
         <f>E13</f>
-        <v>trezentos e um reais e sessenta centavos</v>
-      </c>
-      <c r="F34" s="59"/>
-      <c r="G34" s="59"/>
-      <c r="H34" s="59"/>
-      <c r="I34" s="59"/>
-      <c r="J34" s="59"/>
-      <c r="K34" s="59"/>
-      <c r="L34" s="59"/>
-      <c r="M34" s="60"/>
-      <c r="N34" s="79"/>
+        <v/>
+      </c>
+      <c r="F34" s="81"/>
+      <c r="G34" s="81"/>
+      <c r="H34" s="81"/>
+      <c r="I34" s="81"/>
+      <c r="J34" s="81"/>
+      <c r="K34" s="81"/>
+      <c r="L34" s="81"/>
+      <c r="M34" s="82"/>
+      <c r="N34" s="53"/>
     </row>
     <row r="35" spans="3:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C35" s="77"/>
+      <c r="C35" s="52"/>
       <c r="D35" s="43" t="s">
         <v>95</v>
       </c>
-      <c r="E35" s="61" t="str">
+      <c r="E35" s="83" t="str">
         <f>E14</f>
-        <v>Vale Transporte do mês de Janeiro de 2017. Comtenplando os dias abaixo:</v>
-      </c>
-      <c r="F35" s="61"/>
-      <c r="G35" s="61"/>
-      <c r="H35" s="61"/>
-      <c r="I35" s="61"/>
-      <c r="J35" s="61"/>
-      <c r="K35" s="61"/>
-      <c r="L35" s="61"/>
-      <c r="M35" s="61"/>
-      <c r="N35" s="79"/>
+        <v>Vale Transporte do mês de  de . Comtenplando os dias abaixo:</v>
+      </c>
+      <c r="F35" s="83"/>
+      <c r="G35" s="83"/>
+      <c r="H35" s="83"/>
+      <c r="I35" s="83"/>
+      <c r="J35" s="83"/>
+      <c r="K35" s="83"/>
+      <c r="L35" s="83"/>
+      <c r="M35" s="83"/>
+      <c r="N35" s="53"/>
     </row>
     <row r="36" spans="3:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C36" s="77"/>
-      <c r="D36" s="62" t="str">
+      <c r="C36" s="52"/>
+      <c r="D36" s="77" t="str">
         <f>D15</f>
-        <v>=== / 02-jan-2017 / 03-jan-2017 / 04-jan-2017 / 05-jan-2017 / 06-jan-2017 / 07-jan-2017===</v>
-      </c>
-      <c r="E36" s="63"/>
-      <c r="F36" s="63"/>
-      <c r="G36" s="63"/>
-      <c r="H36" s="63"/>
-      <c r="I36" s="63"/>
-      <c r="J36" s="63"/>
-      <c r="K36" s="63"/>
-      <c r="L36" s="63"/>
-      <c r="M36" s="64"/>
-      <c r="N36" s="79"/>
+        <v>======</v>
+      </c>
+      <c r="E36" s="78"/>
+      <c r="F36" s="78"/>
+      <c r="G36" s="78"/>
+      <c r="H36" s="78"/>
+      <c r="I36" s="78"/>
+      <c r="J36" s="78"/>
+      <c r="K36" s="78"/>
+      <c r="L36" s="78"/>
+      <c r="M36" s="79"/>
+      <c r="N36" s="53"/>
     </row>
     <row r="37" spans="3:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C37" s="77"/>
-      <c r="D37" s="62" t="str">
+      <c r="C37" s="52"/>
+      <c r="D37" s="77" t="str">
         <f>D16</f>
-        <v>==== / 09-jan-2017 / 10-jan-2017 / 11-jan-2017 / 12-jan-2017 / 13-jan-2017 / 14-jan-2017===</v>
-      </c>
-      <c r="E37" s="63"/>
-      <c r="F37" s="63"/>
-      <c r="G37" s="63"/>
-      <c r="H37" s="63"/>
-      <c r="I37" s="63"/>
-      <c r="J37" s="63"/>
-      <c r="K37" s="63"/>
-      <c r="L37" s="63"/>
-      <c r="M37" s="64"/>
-      <c r="N37" s="79"/>
+        <v>=======</v>
+      </c>
+      <c r="E37" s="78"/>
+      <c r="F37" s="78"/>
+      <c r="G37" s="78"/>
+      <c r="H37" s="78"/>
+      <c r="I37" s="78"/>
+      <c r="J37" s="78"/>
+      <c r="K37" s="78"/>
+      <c r="L37" s="78"/>
+      <c r="M37" s="79"/>
+      <c r="N37" s="53"/>
     </row>
     <row r="38" spans="3:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C38" s="77"/>
-      <c r="D38" s="62" t="str">
+      <c r="C38" s="52"/>
+      <c r="D38" s="77" t="str">
         <f>D17</f>
-        <v>=== / 16-jan-2017 / 17-jan-2017 / 18-jan-2017 / 19-jan-2017 / 20-jan-2017 / 21-jan-2017===</v>
-      </c>
-      <c r="E38" s="63"/>
-      <c r="F38" s="63"/>
-      <c r="G38" s="63"/>
-      <c r="H38" s="63"/>
-      <c r="I38" s="63"/>
-      <c r="J38" s="63"/>
-      <c r="K38" s="63"/>
-      <c r="L38" s="63"/>
-      <c r="M38" s="64"/>
-      <c r="N38" s="79"/>
+        <v>======</v>
+      </c>
+      <c r="E38" s="78"/>
+      <c r="F38" s="78"/>
+      <c r="G38" s="78"/>
+      <c r="H38" s="78"/>
+      <c r="I38" s="78"/>
+      <c r="J38" s="78"/>
+      <c r="K38" s="78"/>
+      <c r="L38" s="78"/>
+      <c r="M38" s="79"/>
+      <c r="N38" s="53"/>
     </row>
     <row r="39" spans="3:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C39" s="77"/>
-      <c r="D39" s="62" t="str">
+      <c r="C39" s="52"/>
+      <c r="D39" s="77" t="str">
         <f>D18</f>
-        <v>===/23-jan-2017/24-jan-2017/25-jan-2017/26-jan-2017/27-jan-2017/28-jan-2017===</v>
-      </c>
-      <c r="E39" s="63"/>
-      <c r="F39" s="63"/>
-      <c r="G39" s="63"/>
-      <c r="H39" s="63"/>
-      <c r="I39" s="63"/>
-      <c r="J39" s="63"/>
-      <c r="K39" s="63"/>
-      <c r="L39" s="63"/>
-      <c r="M39" s="64"/>
-      <c r="N39" s="79"/>
+        <v>======</v>
+      </c>
+      <c r="E39" s="78"/>
+      <c r="F39" s="78"/>
+      <c r="G39" s="78"/>
+      <c r="H39" s="78"/>
+      <c r="I39" s="78"/>
+      <c r="J39" s="78"/>
+      <c r="K39" s="78"/>
+      <c r="L39" s="78"/>
+      <c r="M39" s="79"/>
+      <c r="N39" s="53"/>
     </row>
     <row r="40" spans="3:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C40" s="77"/>
-      <c r="D40" s="62" t="str">
+      <c r="C40" s="52"/>
+      <c r="D40" s="77" t="str">
         <f>D19</f>
-        <v>===/30-jan-2017/31-jan-2017===</v>
-      </c>
-      <c r="E40" s="63"/>
-      <c r="F40" s="63"/>
-      <c r="G40" s="63"/>
-      <c r="H40" s="63"/>
-      <c r="I40" s="63"/>
-      <c r="J40" s="63"/>
-      <c r="K40" s="63"/>
-      <c r="L40" s="63"/>
-      <c r="M40" s="64"/>
-      <c r="N40" s="79"/>
+        <v>======</v>
+      </c>
+      <c r="E40" s="78"/>
+      <c r="F40" s="78"/>
+      <c r="G40" s="78"/>
+      <c r="H40" s="78"/>
+      <c r="I40" s="78"/>
+      <c r="J40" s="78"/>
+      <c r="K40" s="78"/>
+      <c r="L40" s="78"/>
+      <c r="M40" s="79"/>
+      <c r="N40" s="53"/>
     </row>
     <row r="41" spans="3:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C41" s="77"/>
-      <c r="D41" s="80"/>
-      <c r="E41" s="81"/>
-      <c r="F41" s="81"/>
-      <c r="G41" s="81"/>
-      <c r="H41" s="81"/>
-      <c r="I41" s="81"/>
-      <c r="J41" s="81"/>
-      <c r="K41" s="81"/>
-      <c r="L41" s="81"/>
-      <c r="M41" s="81"/>
-      <c r="N41" s="79"/>
+      <c r="C41" s="52"/>
+      <c r="D41" s="54"/>
+      <c r="E41" s="55"/>
+      <c r="F41" s="55"/>
+      <c r="G41" s="55"/>
+      <c r="H41" s="55"/>
+      <c r="I41" s="55"/>
+      <c r="J41" s="55"/>
+      <c r="K41" s="55"/>
+      <c r="L41" s="55"/>
+      <c r="M41" s="55"/>
+      <c r="N41" s="53"/>
     </row>
     <row r="42" spans="3:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C42" s="77"/>
-      <c r="D42" s="82" t="str">
+      <c r="C42" s="52"/>
+      <c r="D42" s="56" t="str">
         <f ca="1">D21</f>
-        <v>Brasília, 06 de janeiro de 2017.</v>
-      </c>
-      <c r="E42" s="81"/>
-      <c r="F42" s="81"/>
-      <c r="G42" s="81"/>
-      <c r="H42" s="81"/>
-      <c r="I42" s="81"/>
-      <c r="J42" s="81"/>
-      <c r="K42" s="81"/>
-      <c r="L42" s="81"/>
-      <c r="M42" s="81"/>
-      <c r="N42" s="79"/>
+        <v>Brasília, 24 de fevereiro de 2017.</v>
+      </c>
+      <c r="E42" s="55"/>
+      <c r="F42" s="55"/>
+      <c r="G42" s="55"/>
+      <c r="H42" s="55"/>
+      <c r="I42" s="55"/>
+      <c r="J42" s="55"/>
+      <c r="K42" s="55"/>
+      <c r="L42" s="55"/>
+      <c r="M42" s="55"/>
+      <c r="N42" s="53"/>
     </row>
     <row r="43" spans="3:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C43" s="77"/>
-      <c r="D43" s="80"/>
-      <c r="E43" s="81"/>
-      <c r="F43" s="81"/>
-      <c r="G43" s="81"/>
-      <c r="H43" s="81"/>
-      <c r="I43" s="81"/>
-      <c r="J43" s="81"/>
-      <c r="K43" s="81"/>
-      <c r="L43" s="81"/>
-      <c r="M43" s="81"/>
-      <c r="N43" s="79"/>
+      <c r="C43" s="52"/>
+      <c r="D43" s="54"/>
+      <c r="E43" s="55"/>
+      <c r="F43" s="55"/>
+      <c r="G43" s="55"/>
+      <c r="H43" s="55"/>
+      <c r="I43" s="55"/>
+      <c r="J43" s="55"/>
+      <c r="K43" s="55"/>
+      <c r="L43" s="55"/>
+      <c r="M43" s="55"/>
+      <c r="N43" s="53"/>
     </row>
     <row r="44" spans="3:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C44" s="77"/>
+      <c r="C44" s="52"/>
       <c r="D44" s="43" t="s">
         <v>100</v>
       </c>
-      <c r="E44" s="58" t="str">
+      <c r="E44" s="80" t="str">
         <f>E23</f>
         <v>Mary Green</v>
       </c>
-      <c r="F44" s="59"/>
-      <c r="G44" s="59"/>
-      <c r="H44" s="59"/>
-      <c r="I44" s="60"/>
+      <c r="F44" s="81"/>
+      <c r="G44" s="81"/>
+      <c r="H44" s="81"/>
+      <c r="I44" s="82"/>
       <c r="J44" s="43" t="s">
         <v>101</v>
       </c>
-      <c r="K44" s="59" t="str">
+      <c r="K44" s="81" t="str">
         <f>K23</f>
         <v>123.456.789-99</v>
       </c>
-      <c r="L44" s="59"/>
-      <c r="M44" s="60"/>
-      <c r="N44" s="79"/>
+      <c r="L44" s="81"/>
+      <c r="M44" s="82"/>
+      <c r="N44" s="53"/>
     </row>
     <row r="45" spans="3:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C45" s="77"/>
+      <c r="C45" s="52"/>
       <c r="D45" s="43" t="s">
         <v>94</v>
       </c>
-      <c r="E45" s="61" t="str">
+      <c r="E45" s="83" t="str">
         <f>E24</f>
         <v>Rua xyz, Qd. Z, Lt. Y, Setor Rincon Park Ceul Brasília -DF</v>
       </c>
-      <c r="F45" s="61"/>
-      <c r="G45" s="61"/>
-      <c r="H45" s="61"/>
-      <c r="I45" s="61"/>
-      <c r="J45" s="61"/>
-      <c r="K45" s="61"/>
-      <c r="L45" s="61"/>
-      <c r="M45" s="61"/>
-      <c r="N45" s="79"/>
+      <c r="F45" s="83"/>
+      <c r="G45" s="83"/>
+      <c r="H45" s="83"/>
+      <c r="I45" s="83"/>
+      <c r="J45" s="83"/>
+      <c r="K45" s="83"/>
+      <c r="L45" s="83"/>
+      <c r="M45" s="83"/>
+      <c r="N45" s="53"/>
     </row>
     <row r="46" spans="3:14" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="C46" s="77"/>
+      <c r="C46" s="52"/>
       <c r="D46" s="44" t="s">
         <v>102</v>
       </c>
-      <c r="E46" s="51"/>
-      <c r="F46" s="51"/>
-      <c r="G46" s="51"/>
-      <c r="H46" s="51"/>
-      <c r="I46" s="51"/>
-      <c r="J46" s="51"/>
-      <c r="K46" s="51"/>
-      <c r="L46" s="51"/>
-      <c r="M46" s="51"/>
-      <c r="N46" s="79"/>
+      <c r="E46" s="84"/>
+      <c r="F46" s="84"/>
+      <c r="G46" s="84"/>
+      <c r="H46" s="84"/>
+      <c r="I46" s="84"/>
+      <c r="J46" s="84"/>
+      <c r="K46" s="84"/>
+      <c r="L46" s="84"/>
+      <c r="M46" s="84"/>
+      <c r="N46" s="53"/>
     </row>
     <row r="47" spans="3:14" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C47" s="93"/>
-      <c r="D47" s="94"/>
-      <c r="E47" s="95"/>
-      <c r="F47" s="95"/>
-      <c r="G47" s="95"/>
-      <c r="H47" s="95"/>
-      <c r="I47" s="95"/>
-      <c r="J47" s="95"/>
-      <c r="K47" s="95"/>
-      <c r="L47" s="95"/>
-      <c r="M47" s="95"/>
-      <c r="N47" s="96"/>
+      <c r="C47" s="67"/>
+      <c r="D47" s="68"/>
+      <c r="E47" s="69"/>
+      <c r="F47" s="69"/>
+      <c r="G47" s="69"/>
+      <c r="H47" s="69"/>
+      <c r="I47" s="69"/>
+      <c r="J47" s="69"/>
+      <c r="K47" s="69"/>
+      <c r="L47" s="69"/>
+      <c r="M47" s="69"/>
+      <c r="N47" s="70"/>
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="D19:M19"/>
-    <mergeCell ref="D40:M40"/>
-    <mergeCell ref="D38:M38"/>
-    <mergeCell ref="E44:I44"/>
-    <mergeCell ref="K44:M44"/>
+    <mergeCell ref="D18:M18"/>
+    <mergeCell ref="D17:M17"/>
+    <mergeCell ref="E12:M12"/>
+    <mergeCell ref="E14:M14"/>
+    <mergeCell ref="E13:M13"/>
+    <mergeCell ref="D15:M15"/>
+    <mergeCell ref="D16:M16"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="D7:M7"/>
+    <mergeCell ref="E11:M11"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="D1:I1"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
     <mergeCell ref="E45:M45"/>
     <mergeCell ref="E46:M46"/>
     <mergeCell ref="D39:M39"/>
@@ -4611,34 +4608,20 @@
     <mergeCell ref="E35:M35"/>
     <mergeCell ref="D36:M36"/>
     <mergeCell ref="D37:M37"/>
+    <mergeCell ref="D19:M19"/>
+    <mergeCell ref="D40:M40"/>
+    <mergeCell ref="D38:M38"/>
+    <mergeCell ref="E44:I44"/>
+    <mergeCell ref="K44:M44"/>
     <mergeCell ref="D28:M28"/>
     <mergeCell ref="E30:F30"/>
     <mergeCell ref="J30:K30"/>
     <mergeCell ref="L30:M30"/>
     <mergeCell ref="E32:M32"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="F3:I3"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="D1:I1"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D4:E4"/>
     <mergeCell ref="E25:M25"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="D7:M7"/>
-    <mergeCell ref="E11:M11"/>
     <mergeCell ref="E24:M24"/>
     <mergeCell ref="K23:M23"/>
     <mergeCell ref="E23:I23"/>
-    <mergeCell ref="D17:M17"/>
-    <mergeCell ref="E12:M12"/>
-    <mergeCell ref="E14:M14"/>
-    <mergeCell ref="E13:M13"/>
-    <mergeCell ref="D15:M15"/>
-    <mergeCell ref="D16:M16"/>
-    <mergeCell ref="D18:M18"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3">
@@ -4695,7 +4678,7 @@
       <c r="A4" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B4" s="97" t="s">
+      <c r="B4" s="71" t="s">
         <v>105</v>
       </c>
     </row>

</xml_diff>